<commit_message>
Afegida indexació confirmacions any 1804
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Confirmacions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084226F7-ECC3-4BF2-A41E-D42699A15F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F3CDCE-C534-4EFE-A0BF-1893F7E08655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FEEAE0F-87B7-4CFD-9217-CD5D622A9875}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4153" uniqueCount="912">
   <si>
     <t>Cognons</t>
   </si>
@@ -2497,6 +2497,285 @@
   </si>
   <si>
     <t>Pujades Vallés Caterina</t>
+  </si>
+  <si>
+    <t>Pedrós Querol Jaume</t>
+  </si>
+  <si>
+    <t>Ortiz Vila Jaume</t>
+  </si>
+  <si>
+    <t>Escolà Espinal Josep</t>
+  </si>
+  <si>
+    <t>Coll Sunyé Francisco</t>
+  </si>
+  <si>
+    <t>Gasol Tort Francisca</t>
+  </si>
+  <si>
+    <t>Balcells Roig Francisca</t>
+  </si>
+  <si>
+    <t>Majoral Tarragó Francisca</t>
+  </si>
+  <si>
+    <t>Oriol Enguese Rosa</t>
+  </si>
+  <si>
+    <t>Querol Massà Antonia</t>
+  </si>
+  <si>
+    <t>Mas Corbella Dolors</t>
+  </si>
+  <si>
+    <t>Mas Macià Josep</t>
+  </si>
+  <si>
+    <t>Castelló Riba Magi</t>
+  </si>
+  <si>
+    <t>Galitó Majoral Josep</t>
+  </si>
+  <si>
+    <t>Pedrós Balagué Rosa</t>
+  </si>
+  <si>
+    <t>Padulles Martí Palmira</t>
+  </si>
+  <si>
+    <t>Domingo Renye Josepa</t>
+  </si>
+  <si>
+    <t>Badia Solé Rafael</t>
+  </si>
+  <si>
+    <t>Piulats Gispert Maria</t>
+  </si>
+  <si>
+    <t>Sole Coll Josep Maria</t>
+  </si>
+  <si>
+    <t>Bonjorn Huguet Teresa</t>
+  </si>
+  <si>
+    <t>Llanes Gili Francisco</t>
+  </si>
+  <si>
+    <t>Vilaplana Domenjo Eusebi</t>
+  </si>
+  <si>
+    <t>Mas Camarasa Maria</t>
+  </si>
+  <si>
+    <t>Cisteré Galceran Francisco</t>
+  </si>
+  <si>
+    <t>Solé Vergé Ramon</t>
+  </si>
+  <si>
+    <t>Plà Coll Manuela</t>
+  </si>
+  <si>
+    <t>Torrades Oliva Estanislao</t>
+  </si>
+  <si>
+    <t>Torrades Oliva Ramon</t>
+  </si>
+  <si>
+    <t>Bonjorn Camprubí Eloi</t>
+  </si>
+  <si>
+    <t>Trepat Trepat Ramon</t>
+  </si>
+  <si>
+    <t>Giné Pedrós Francisco</t>
+  </si>
+  <si>
+    <t>Saball Chuclà Rosa</t>
+  </si>
+  <si>
+    <t>Majoral Pujoil Esteve</t>
+  </si>
+  <si>
+    <t>Seball Xuvlà Miquel</t>
+  </si>
+  <si>
+    <t>Gasol Tort Rosa</t>
+  </si>
+  <si>
+    <t>Palou Civit Josep</t>
+  </si>
+  <si>
+    <t>Pujades Coll Teresa</t>
+  </si>
+  <si>
+    <t>Bosch Galceran Concepció</t>
+  </si>
+  <si>
+    <t>Planes Mauri Jaume</t>
+  </si>
+  <si>
+    <t>Balasch Torrent Cecilia</t>
+  </si>
+  <si>
+    <t>Saball Xuclà Secundina</t>
+  </si>
+  <si>
+    <t>Colell Pujades Andreu</t>
+  </si>
+  <si>
+    <t>Solsona Llovera Ramon</t>
+  </si>
+  <si>
+    <t>Duart Pallerola María</t>
+  </si>
+  <si>
+    <t>Bosch Galceran Josepa</t>
+  </si>
+  <si>
+    <t>Roma Majoral Francisco</t>
+  </si>
+  <si>
+    <t>Tacies Cunyat Francisco</t>
+  </si>
+  <si>
+    <t>Roca Sans Jaume</t>
+  </si>
+  <si>
+    <t>Gispert Segarra Regina</t>
+  </si>
+  <si>
+    <t>Ortiz Vila Joan</t>
+  </si>
+  <si>
+    <t>Oliva Figuera Antonia</t>
+  </si>
+  <si>
+    <t>Oliva Figuera Maria</t>
+  </si>
+  <si>
+    <t>Gili Pons Agustí</t>
+  </si>
+  <si>
+    <t>Colell Majoral Francisco</t>
+  </si>
+  <si>
+    <t>Vives Morera Rosa</t>
+  </si>
+  <si>
+    <t>Balcells Pedrós Francisco</t>
+  </si>
+  <si>
+    <t>Vilamajó Pallàs Domingo</t>
+  </si>
+  <si>
+    <t>Pedrós Querol Antonia</t>
+  </si>
+  <si>
+    <t>Gispert Segarra Margarita</t>
+  </si>
+  <si>
+    <t>Majoral Vergé Dolors</t>
+  </si>
+  <si>
+    <t>Eroles Majoral Manuel</t>
+  </si>
+  <si>
+    <t>Eroles Majoral Josep</t>
+  </si>
+  <si>
+    <t>Colell Pujades Josep</t>
+  </si>
+  <si>
+    <t>Mas Combella Arnengol</t>
+  </si>
+  <si>
+    <t>Massana Boldú Josep</t>
+  </si>
+  <si>
+    <t>Bonjorn Pedrós Maria</t>
+  </si>
+  <si>
+    <t>Solé Rubies Antonio</t>
+  </si>
+  <si>
+    <t>Binefa Torrent Antonia</t>
+  </si>
+  <si>
+    <t>Marti Plassa Joan</t>
+  </si>
+  <si>
+    <t>Gispert Segarra Erminia</t>
+  </si>
+  <si>
+    <t>Mas Gené Andres</t>
+  </si>
+  <si>
+    <t>Solé Rubies Teresa</t>
+  </si>
+  <si>
+    <t>Cascalló Ribes Trinidad</t>
+  </si>
+  <si>
+    <t>Gené Marti Josep</t>
+  </si>
+  <si>
+    <t>Gene Marti Rosa</t>
+  </si>
+  <si>
+    <t>Riera Palou Rafael</t>
+  </si>
+  <si>
+    <t>Foguet Arderiu Manuela</t>
+  </si>
+  <si>
+    <t>Mas Gispert Rosa</t>
+  </si>
+  <si>
+    <t>Gispert Martí Elisa?</t>
+  </si>
+  <si>
+    <t>Coll Sunyé Dolors</t>
+  </si>
+  <si>
+    <t>Velimelis Pedra Roc</t>
+  </si>
+  <si>
+    <t>Farré Castelló Maria</t>
+  </si>
+  <si>
+    <t>Palau Tarragó Dolors</t>
+  </si>
+  <si>
+    <t>Mosset Arbós Rosa</t>
+  </si>
+  <si>
+    <t>Majoral Pedrós Consol</t>
+  </si>
+  <si>
+    <t>Roca Sans Josep</t>
+  </si>
+  <si>
+    <t>Domenjó Renyé Amparo</t>
+  </si>
+  <si>
+    <t>Vilamajó Oakkes Sebastian</t>
+  </si>
+  <si>
+    <t>Bosch Galceran Ramon</t>
+  </si>
+  <si>
+    <t>Palau Tarragó María</t>
+  </si>
+  <si>
+    <t>Gené Trepat Josep</t>
+  </si>
+  <si>
+    <t>Paul Castarleuas? Antonia</t>
+  </si>
+  <si>
+    <t>Ginestà Borrell Ramon</t>
   </si>
 </sst>
 </file>
@@ -2862,10 +3141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EAC519-AAA9-4752-A1C1-63CDDDDDC53A}">
-  <dimension ref="A1:L794"/>
+  <dimension ref="A1:L887"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A775" workbookViewId="0">
-      <selection activeCell="A795" sqref="A795"/>
+    <sheetView tabSelected="1" topLeftCell="A855" workbookViewId="0">
+      <selection activeCell="E883" sqref="E883"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25276,6 +25555,2424 @@
         <v>12</v>
       </c>
       <c r="K794" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="795" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A795">
+        <v>54</v>
+      </c>
+      <c r="B795">
+        <v>1804</v>
+      </c>
+      <c r="C795" t="s">
+        <v>819</v>
+      </c>
+      <c r="F795" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H795" t="s">
+        <v>11</v>
+      </c>
+      <c r="I795">
+        <v>47</v>
+      </c>
+      <c r="J795" t="s">
+        <v>12</v>
+      </c>
+      <c r="K795" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="796" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A796">
+        <v>54</v>
+      </c>
+      <c r="B796">
+        <v>1804</v>
+      </c>
+      <c r="C796" t="s">
+        <v>820</v>
+      </c>
+      <c r="F796" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H796" t="s">
+        <v>11</v>
+      </c>
+      <c r="I796">
+        <v>47</v>
+      </c>
+      <c r="J796" t="s">
+        <v>12</v>
+      </c>
+      <c r="K796" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="797" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A797">
+        <v>54</v>
+      </c>
+      <c r="B797">
+        <v>1804</v>
+      </c>
+      <c r="C797" t="s">
+        <v>821</v>
+      </c>
+      <c r="F797" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H797" t="s">
+        <v>11</v>
+      </c>
+      <c r="I797">
+        <v>47</v>
+      </c>
+      <c r="J797" t="s">
+        <v>12</v>
+      </c>
+      <c r="K797" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="798" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A798">
+        <v>54</v>
+      </c>
+      <c r="B798">
+        <v>1804</v>
+      </c>
+      <c r="C798" t="s">
+        <v>822</v>
+      </c>
+      <c r="F798" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H798" t="s">
+        <v>11</v>
+      </c>
+      <c r="I798">
+        <v>47</v>
+      </c>
+      <c r="J798" t="s">
+        <v>12</v>
+      </c>
+      <c r="K798" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="799" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A799">
+        <v>54</v>
+      </c>
+      <c r="B799">
+        <v>1804</v>
+      </c>
+      <c r="C799" t="s">
+        <v>823</v>
+      </c>
+      <c r="F799" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H799" t="s">
+        <v>11</v>
+      </c>
+      <c r="I799">
+        <v>47</v>
+      </c>
+      <c r="J799" t="s">
+        <v>12</v>
+      </c>
+      <c r="K799" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="800" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A800">
+        <v>54</v>
+      </c>
+      <c r="B800">
+        <v>1804</v>
+      </c>
+      <c r="C800" t="s">
+        <v>824</v>
+      </c>
+      <c r="F800" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H800" t="s">
+        <v>11</v>
+      </c>
+      <c r="I800">
+        <v>47</v>
+      </c>
+      <c r="J800" t="s">
+        <v>12</v>
+      </c>
+      <c r="K800" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="801" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A801">
+        <v>54</v>
+      </c>
+      <c r="B801">
+        <v>1804</v>
+      </c>
+      <c r="C801" t="s">
+        <v>825</v>
+      </c>
+      <c r="F801" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H801" t="s">
+        <v>11</v>
+      </c>
+      <c r="I801">
+        <v>47</v>
+      </c>
+      <c r="J801" t="s">
+        <v>12</v>
+      </c>
+      <c r="K801" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="802" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A802">
+        <v>54</v>
+      </c>
+      <c r="B802">
+        <v>1804</v>
+      </c>
+      <c r="C802" t="s">
+        <v>826</v>
+      </c>
+      <c r="F802" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H802" t="s">
+        <v>11</v>
+      </c>
+      <c r="I802">
+        <v>47</v>
+      </c>
+      <c r="J802" t="s">
+        <v>12</v>
+      </c>
+      <c r="K802" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="803" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A803">
+        <v>54</v>
+      </c>
+      <c r="B803">
+        <v>1804</v>
+      </c>
+      <c r="C803" t="s">
+        <v>827</v>
+      </c>
+      <c r="F803" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H803" t="s">
+        <v>11</v>
+      </c>
+      <c r="I803">
+        <v>47</v>
+      </c>
+      <c r="J803" t="s">
+        <v>12</v>
+      </c>
+      <c r="K803" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="804" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A804">
+        <v>54</v>
+      </c>
+      <c r="B804">
+        <v>1804</v>
+      </c>
+      <c r="C804" t="s">
+        <v>828</v>
+      </c>
+      <c r="F804" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H804" t="s">
+        <v>11</v>
+      </c>
+      <c r="I804">
+        <v>47</v>
+      </c>
+      <c r="J804" t="s">
+        <v>12</v>
+      </c>
+      <c r="K804" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="805" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A805">
+        <v>54</v>
+      </c>
+      <c r="B805">
+        <v>1804</v>
+      </c>
+      <c r="C805" t="s">
+        <v>829</v>
+      </c>
+      <c r="F805" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H805" t="s">
+        <v>11</v>
+      </c>
+      <c r="I805">
+        <v>47</v>
+      </c>
+      <c r="J805" t="s">
+        <v>12</v>
+      </c>
+      <c r="K805" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="806" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A806">
+        <v>54</v>
+      </c>
+      <c r="B806">
+        <v>1804</v>
+      </c>
+      <c r="C806" t="s">
+        <v>830</v>
+      </c>
+      <c r="F806" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H806" t="s">
+        <v>11</v>
+      </c>
+      <c r="I806">
+        <v>47</v>
+      </c>
+      <c r="J806" t="s">
+        <v>12</v>
+      </c>
+      <c r="K806" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="807" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A807">
+        <v>54</v>
+      </c>
+      <c r="B807">
+        <v>1804</v>
+      </c>
+      <c r="C807" t="s">
+        <v>831</v>
+      </c>
+      <c r="F807" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H807" t="s">
+        <v>11</v>
+      </c>
+      <c r="I807">
+        <v>47</v>
+      </c>
+      <c r="J807" t="s">
+        <v>12</v>
+      </c>
+      <c r="K807" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="808" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A808">
+        <v>54</v>
+      </c>
+      <c r="B808">
+        <v>1804</v>
+      </c>
+      <c r="C808" t="s">
+        <v>832</v>
+      </c>
+      <c r="F808" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H808" t="s">
+        <v>11</v>
+      </c>
+      <c r="I808">
+        <v>47</v>
+      </c>
+      <c r="J808" t="s">
+        <v>12</v>
+      </c>
+      <c r="K808" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="809" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A809">
+        <v>54</v>
+      </c>
+      <c r="B809">
+        <v>1804</v>
+      </c>
+      <c r="C809" t="s">
+        <v>833</v>
+      </c>
+      <c r="F809" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H809" t="s">
+        <v>11</v>
+      </c>
+      <c r="I809">
+        <v>47</v>
+      </c>
+      <c r="J809" t="s">
+        <v>12</v>
+      </c>
+      <c r="K809" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="810" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A810">
+        <v>54</v>
+      </c>
+      <c r="B810">
+        <v>1804</v>
+      </c>
+      <c r="C810" t="s">
+        <v>834</v>
+      </c>
+      <c r="F810" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H810" t="s">
+        <v>11</v>
+      </c>
+      <c r="I810">
+        <v>47</v>
+      </c>
+      <c r="J810" t="s">
+        <v>12</v>
+      </c>
+      <c r="K810" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="811" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A811">
+        <v>54</v>
+      </c>
+      <c r="B811">
+        <v>1804</v>
+      </c>
+      <c r="C811" t="s">
+        <v>835</v>
+      </c>
+      <c r="F811" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H811" t="s">
+        <v>11</v>
+      </c>
+      <c r="I811">
+        <v>47</v>
+      </c>
+      <c r="J811" t="s">
+        <v>12</v>
+      </c>
+      <c r="K811" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="812" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A812">
+        <v>54</v>
+      </c>
+      <c r="B812">
+        <v>1804</v>
+      </c>
+      <c r="C812" t="s">
+        <v>836</v>
+      </c>
+      <c r="F812" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H812" t="s">
+        <v>11</v>
+      </c>
+      <c r="I812">
+        <v>47</v>
+      </c>
+      <c r="J812" t="s">
+        <v>12</v>
+      </c>
+      <c r="K812" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="813" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A813">
+        <v>54</v>
+      </c>
+      <c r="B813">
+        <v>1804</v>
+      </c>
+      <c r="C813" t="s">
+        <v>837</v>
+      </c>
+      <c r="F813" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H813" t="s">
+        <v>11</v>
+      </c>
+      <c r="I813">
+        <v>47</v>
+      </c>
+      <c r="J813" t="s">
+        <v>12</v>
+      </c>
+      <c r="K813" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="814" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A814">
+        <v>54</v>
+      </c>
+      <c r="B814">
+        <v>1804</v>
+      </c>
+      <c r="C814" t="s">
+        <v>838</v>
+      </c>
+      <c r="F814" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H814" t="s">
+        <v>11</v>
+      </c>
+      <c r="I814">
+        <v>47</v>
+      </c>
+      <c r="J814" t="s">
+        <v>12</v>
+      </c>
+      <c r="K814" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="815" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A815">
+        <v>54</v>
+      </c>
+      <c r="B815">
+        <v>1804</v>
+      </c>
+      <c r="C815" t="s">
+        <v>839</v>
+      </c>
+      <c r="F815" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H815" t="s">
+        <v>11</v>
+      </c>
+      <c r="I815">
+        <v>47</v>
+      </c>
+      <c r="J815" t="s">
+        <v>12</v>
+      </c>
+      <c r="K815" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="816" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A816">
+        <v>54</v>
+      </c>
+      <c r="B816">
+        <v>1804</v>
+      </c>
+      <c r="C816" t="s">
+        <v>840</v>
+      </c>
+      <c r="F816" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H816" t="s">
+        <v>11</v>
+      </c>
+      <c r="I816">
+        <v>47</v>
+      </c>
+      <c r="J816" t="s">
+        <v>12</v>
+      </c>
+      <c r="K816" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="817" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A817">
+        <v>54</v>
+      </c>
+      <c r="B817">
+        <v>1804</v>
+      </c>
+      <c r="C817" t="s">
+        <v>841</v>
+      </c>
+      <c r="F817" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H817" t="s">
+        <v>11</v>
+      </c>
+      <c r="I817">
+        <v>47</v>
+      </c>
+      <c r="J817" t="s">
+        <v>12</v>
+      </c>
+      <c r="K817" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="818" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A818">
+        <v>54</v>
+      </c>
+      <c r="B818">
+        <v>1804</v>
+      </c>
+      <c r="C818" t="s">
+        <v>842</v>
+      </c>
+      <c r="F818" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H818" t="s">
+        <v>11</v>
+      </c>
+      <c r="I818">
+        <v>47</v>
+      </c>
+      <c r="J818" t="s">
+        <v>12</v>
+      </c>
+      <c r="K818" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="819" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A819">
+        <v>54</v>
+      </c>
+      <c r="B819">
+        <v>1804</v>
+      </c>
+      <c r="C819" t="s">
+        <v>843</v>
+      </c>
+      <c r="F819" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H819" t="s">
+        <v>11</v>
+      </c>
+      <c r="I819">
+        <v>47</v>
+      </c>
+      <c r="J819" t="s">
+        <v>12</v>
+      </c>
+      <c r="K819" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="820" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A820">
+        <v>54</v>
+      </c>
+      <c r="B820">
+        <v>1804</v>
+      </c>
+      <c r="C820" t="s">
+        <v>844</v>
+      </c>
+      <c r="F820" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H820" t="s">
+        <v>11</v>
+      </c>
+      <c r="I820">
+        <v>47</v>
+      </c>
+      <c r="J820" t="s">
+        <v>12</v>
+      </c>
+      <c r="K820" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="821" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A821">
+        <v>54</v>
+      </c>
+      <c r="B821">
+        <v>1804</v>
+      </c>
+      <c r="C821" t="s">
+        <v>845</v>
+      </c>
+      <c r="F821" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H821" t="s">
+        <v>11</v>
+      </c>
+      <c r="I821">
+        <v>47</v>
+      </c>
+      <c r="J821" t="s">
+        <v>12</v>
+      </c>
+      <c r="K821" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="822" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A822">
+        <v>54</v>
+      </c>
+      <c r="B822">
+        <v>1804</v>
+      </c>
+      <c r="C822" t="s">
+        <v>846</v>
+      </c>
+      <c r="F822" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H822" t="s">
+        <v>11</v>
+      </c>
+      <c r="I822">
+        <v>47</v>
+      </c>
+      <c r="J822" t="s">
+        <v>12</v>
+      </c>
+      <c r="K822" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="823" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A823">
+        <v>54</v>
+      </c>
+      <c r="B823">
+        <v>1804</v>
+      </c>
+      <c r="C823" t="s">
+        <v>847</v>
+      </c>
+      <c r="F823" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H823" t="s">
+        <v>11</v>
+      </c>
+      <c r="I823">
+        <v>47</v>
+      </c>
+      <c r="J823" t="s">
+        <v>12</v>
+      </c>
+      <c r="K823" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="824" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A824">
+        <v>54</v>
+      </c>
+      <c r="B824">
+        <v>1804</v>
+      </c>
+      <c r="C824" t="s">
+        <v>848</v>
+      </c>
+      <c r="F824" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H824" t="s">
+        <v>11</v>
+      </c>
+      <c r="I824">
+        <v>47</v>
+      </c>
+      <c r="J824" t="s">
+        <v>12</v>
+      </c>
+      <c r="K824" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="825" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A825">
+        <v>54</v>
+      </c>
+      <c r="B825">
+        <v>1804</v>
+      </c>
+      <c r="C825" t="s">
+        <v>849</v>
+      </c>
+      <c r="F825" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H825" t="s">
+        <v>11</v>
+      </c>
+      <c r="I825">
+        <v>47</v>
+      </c>
+      <c r="J825" t="s">
+        <v>12</v>
+      </c>
+      <c r="K825" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="826" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A826">
+        <v>54</v>
+      </c>
+      <c r="B826">
+        <v>1804</v>
+      </c>
+      <c r="C826" t="s">
+        <v>850</v>
+      </c>
+      <c r="F826" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H826" t="s">
+        <v>11</v>
+      </c>
+      <c r="I826">
+        <v>47</v>
+      </c>
+      <c r="J826" t="s">
+        <v>12</v>
+      </c>
+      <c r="K826" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="827" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A827">
+        <v>54</v>
+      </c>
+      <c r="B827">
+        <v>1804</v>
+      </c>
+      <c r="C827" t="s">
+        <v>851</v>
+      </c>
+      <c r="F827" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H827" t="s">
+        <v>11</v>
+      </c>
+      <c r="I827">
+        <v>47</v>
+      </c>
+      <c r="J827" t="s">
+        <v>12</v>
+      </c>
+      <c r="K827" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="828" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A828">
+        <v>54</v>
+      </c>
+      <c r="B828">
+        <v>1804</v>
+      </c>
+      <c r="C828" t="s">
+        <v>852</v>
+      </c>
+      <c r="F828" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H828" t="s">
+        <v>11</v>
+      </c>
+      <c r="I828">
+        <v>47</v>
+      </c>
+      <c r="J828" t="s">
+        <v>12</v>
+      </c>
+      <c r="K828" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="829" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A829">
+        <v>54</v>
+      </c>
+      <c r="B829">
+        <v>1804</v>
+      </c>
+      <c r="C829" t="s">
+        <v>853</v>
+      </c>
+      <c r="F829" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H829" t="s">
+        <v>11</v>
+      </c>
+      <c r="I829">
+        <v>47</v>
+      </c>
+      <c r="J829" t="s">
+        <v>12</v>
+      </c>
+      <c r="K829" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="830" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A830">
+        <v>54</v>
+      </c>
+      <c r="B830">
+        <v>1804</v>
+      </c>
+      <c r="C830" t="s">
+        <v>854</v>
+      </c>
+      <c r="F830" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H830" t="s">
+        <v>11</v>
+      </c>
+      <c r="I830">
+        <v>47</v>
+      </c>
+      <c r="J830" t="s">
+        <v>12</v>
+      </c>
+      <c r="K830" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="831" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A831">
+        <v>54</v>
+      </c>
+      <c r="B831">
+        <v>1804</v>
+      </c>
+      <c r="C831" t="s">
+        <v>855</v>
+      </c>
+      <c r="F831" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H831" t="s">
+        <v>11</v>
+      </c>
+      <c r="I831">
+        <v>47</v>
+      </c>
+      <c r="J831" t="s">
+        <v>12</v>
+      </c>
+      <c r="K831" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="832" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A832">
+        <v>54</v>
+      </c>
+      <c r="B832">
+        <v>1804</v>
+      </c>
+      <c r="C832" t="s">
+        <v>856</v>
+      </c>
+      <c r="F832" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H832" t="s">
+        <v>11</v>
+      </c>
+      <c r="I832">
+        <v>47</v>
+      </c>
+      <c r="J832" t="s">
+        <v>12</v>
+      </c>
+      <c r="K832" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="833" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A833">
+        <v>54</v>
+      </c>
+      <c r="B833">
+        <v>1804</v>
+      </c>
+      <c r="C833" t="s">
+        <v>857</v>
+      </c>
+      <c r="F833" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H833" t="s">
+        <v>11</v>
+      </c>
+      <c r="I833">
+        <v>47</v>
+      </c>
+      <c r="J833" t="s">
+        <v>12</v>
+      </c>
+      <c r="K833" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="834" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A834">
+        <v>54</v>
+      </c>
+      <c r="B834">
+        <v>1804</v>
+      </c>
+      <c r="C834" t="s">
+        <v>858</v>
+      </c>
+      <c r="F834" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H834" t="s">
+        <v>11</v>
+      </c>
+      <c r="I834">
+        <v>47</v>
+      </c>
+      <c r="J834" t="s">
+        <v>12</v>
+      </c>
+      <c r="K834" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="835" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A835">
+        <v>54</v>
+      </c>
+      <c r="B835">
+        <v>1804</v>
+      </c>
+      <c r="C835" t="s">
+        <v>859</v>
+      </c>
+      <c r="F835" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H835" t="s">
+        <v>11</v>
+      </c>
+      <c r="I835">
+        <v>47</v>
+      </c>
+      <c r="J835" t="s">
+        <v>12</v>
+      </c>
+      <c r="K835" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="836" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A836">
+        <v>54</v>
+      </c>
+      <c r="B836">
+        <v>1804</v>
+      </c>
+      <c r="C836" t="s">
+        <v>860</v>
+      </c>
+      <c r="F836" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H836" t="s">
+        <v>11</v>
+      </c>
+      <c r="I836">
+        <v>47</v>
+      </c>
+      <c r="J836" t="s">
+        <v>12</v>
+      </c>
+      <c r="K836" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="837" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A837">
+        <v>54</v>
+      </c>
+      <c r="B837">
+        <v>1804</v>
+      </c>
+      <c r="C837" t="s">
+        <v>861</v>
+      </c>
+      <c r="F837" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H837" t="s">
+        <v>11</v>
+      </c>
+      <c r="I837">
+        <v>47</v>
+      </c>
+      <c r="J837" t="s">
+        <v>12</v>
+      </c>
+      <c r="K837" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="838" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A838">
+        <v>54</v>
+      </c>
+      <c r="B838">
+        <v>1804</v>
+      </c>
+      <c r="C838" t="s">
+        <v>862</v>
+      </c>
+      <c r="F838" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H838" t="s">
+        <v>11</v>
+      </c>
+      <c r="I838">
+        <v>47</v>
+      </c>
+      <c r="J838" t="s">
+        <v>12</v>
+      </c>
+      <c r="K838" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="839" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A839">
+        <v>54</v>
+      </c>
+      <c r="B839">
+        <v>1804</v>
+      </c>
+      <c r="C839" t="s">
+        <v>863</v>
+      </c>
+      <c r="F839" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H839" t="s">
+        <v>11</v>
+      </c>
+      <c r="I839">
+        <v>47</v>
+      </c>
+      <c r="J839" t="s">
+        <v>12</v>
+      </c>
+      <c r="K839" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="840" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A840">
+        <v>54</v>
+      </c>
+      <c r="B840">
+        <v>1804</v>
+      </c>
+      <c r="C840" t="s">
+        <v>864</v>
+      </c>
+      <c r="F840" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H840" t="s">
+        <v>11</v>
+      </c>
+      <c r="I840">
+        <v>47</v>
+      </c>
+      <c r="J840" t="s">
+        <v>12</v>
+      </c>
+      <c r="K840" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="841" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A841">
+        <v>54</v>
+      </c>
+      <c r="B841">
+        <v>1804</v>
+      </c>
+      <c r="C841" t="s">
+        <v>865</v>
+      </c>
+      <c r="F841" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H841" t="s">
+        <v>11</v>
+      </c>
+      <c r="I841">
+        <v>47</v>
+      </c>
+      <c r="J841" t="s">
+        <v>12</v>
+      </c>
+      <c r="K841" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="842" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A842">
+        <v>54</v>
+      </c>
+      <c r="B842">
+        <v>1804</v>
+      </c>
+      <c r="C842" t="s">
+        <v>866</v>
+      </c>
+      <c r="F842" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H842" t="s">
+        <v>11</v>
+      </c>
+      <c r="I842">
+        <v>47</v>
+      </c>
+      <c r="J842" t="s">
+        <v>12</v>
+      </c>
+      <c r="K842" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="843" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A843">
+        <v>54</v>
+      </c>
+      <c r="B843">
+        <v>1804</v>
+      </c>
+      <c r="C843" t="s">
+        <v>867</v>
+      </c>
+      <c r="F843" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H843" t="s">
+        <v>11</v>
+      </c>
+      <c r="I843">
+        <v>47</v>
+      </c>
+      <c r="J843" t="s">
+        <v>12</v>
+      </c>
+      <c r="K843" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="844" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A844">
+        <v>54</v>
+      </c>
+      <c r="B844">
+        <v>1804</v>
+      </c>
+      <c r="C844" t="s">
+        <v>868</v>
+      </c>
+      <c r="F844" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H844" t="s">
+        <v>11</v>
+      </c>
+      <c r="I844">
+        <v>47</v>
+      </c>
+      <c r="J844" t="s">
+        <v>12</v>
+      </c>
+      <c r="K844" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="845" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A845">
+        <v>54</v>
+      </c>
+      <c r="B845">
+        <v>1804</v>
+      </c>
+      <c r="C845" t="s">
+        <v>869</v>
+      </c>
+      <c r="F845" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H845" t="s">
+        <v>11</v>
+      </c>
+      <c r="I845">
+        <v>47</v>
+      </c>
+      <c r="J845" t="s">
+        <v>12</v>
+      </c>
+      <c r="K845" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="846" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A846">
+        <v>54</v>
+      </c>
+      <c r="B846">
+        <v>1804</v>
+      </c>
+      <c r="C846" t="s">
+        <v>870</v>
+      </c>
+      <c r="F846" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H846" t="s">
+        <v>11</v>
+      </c>
+      <c r="I846">
+        <v>47</v>
+      </c>
+      <c r="J846" t="s">
+        <v>12</v>
+      </c>
+      <c r="K846" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="847" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A847">
+        <v>54</v>
+      </c>
+      <c r="B847">
+        <v>1804</v>
+      </c>
+      <c r="C847" t="s">
+        <v>871</v>
+      </c>
+      <c r="F847" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H847" t="s">
+        <v>11</v>
+      </c>
+      <c r="I847">
+        <v>47</v>
+      </c>
+      <c r="J847" t="s">
+        <v>12</v>
+      </c>
+      <c r="K847" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="848" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A848">
+        <v>54</v>
+      </c>
+      <c r="B848">
+        <v>1804</v>
+      </c>
+      <c r="C848" t="s">
+        <v>872</v>
+      </c>
+      <c r="F848" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H848" t="s">
+        <v>11</v>
+      </c>
+      <c r="I848">
+        <v>47</v>
+      </c>
+      <c r="J848" t="s">
+        <v>12</v>
+      </c>
+      <c r="K848" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="849" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A849">
+        <v>54</v>
+      </c>
+      <c r="B849">
+        <v>1804</v>
+      </c>
+      <c r="C849" t="s">
+        <v>873</v>
+      </c>
+      <c r="F849" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H849" t="s">
+        <v>11</v>
+      </c>
+      <c r="I849">
+        <v>47</v>
+      </c>
+      <c r="J849" t="s">
+        <v>12</v>
+      </c>
+      <c r="K849" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="850" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A850">
+        <v>54</v>
+      </c>
+      <c r="B850">
+        <v>1804</v>
+      </c>
+      <c r="C850" t="s">
+        <v>874</v>
+      </c>
+      <c r="F850" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H850" t="s">
+        <v>11</v>
+      </c>
+      <c r="I850">
+        <v>47</v>
+      </c>
+      <c r="J850" t="s">
+        <v>12</v>
+      </c>
+      <c r="K850" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="851" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A851">
+        <v>54</v>
+      </c>
+      <c r="B851">
+        <v>1804</v>
+      </c>
+      <c r="C851" t="s">
+        <v>875</v>
+      </c>
+      <c r="F851" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H851" t="s">
+        <v>11</v>
+      </c>
+      <c r="I851">
+        <v>47</v>
+      </c>
+      <c r="J851" t="s">
+        <v>12</v>
+      </c>
+      <c r="K851" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="852" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A852">
+        <v>54</v>
+      </c>
+      <c r="B852">
+        <v>1804</v>
+      </c>
+      <c r="C852" t="s">
+        <v>876</v>
+      </c>
+      <c r="F852" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H852" t="s">
+        <v>11</v>
+      </c>
+      <c r="I852">
+        <v>47</v>
+      </c>
+      <c r="J852" t="s">
+        <v>12</v>
+      </c>
+      <c r="K852" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="853" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A853">
+        <v>54</v>
+      </c>
+      <c r="B853">
+        <v>1804</v>
+      </c>
+      <c r="C853" t="s">
+        <v>877</v>
+      </c>
+      <c r="F853" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H853" t="s">
+        <v>11</v>
+      </c>
+      <c r="I853">
+        <v>47</v>
+      </c>
+      <c r="J853" t="s">
+        <v>12</v>
+      </c>
+      <c r="K853" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="854" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A854">
+        <v>54</v>
+      </c>
+      <c r="B854">
+        <v>1804</v>
+      </c>
+      <c r="C854" t="s">
+        <v>878</v>
+      </c>
+      <c r="F854" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H854" t="s">
+        <v>11</v>
+      </c>
+      <c r="I854">
+        <v>47</v>
+      </c>
+      <c r="J854" t="s">
+        <v>12</v>
+      </c>
+      <c r="K854" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="855" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A855">
+        <v>54</v>
+      </c>
+      <c r="B855">
+        <v>1804</v>
+      </c>
+      <c r="C855" t="s">
+        <v>879</v>
+      </c>
+      <c r="F855" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H855" t="s">
+        <v>11</v>
+      </c>
+      <c r="I855">
+        <v>47</v>
+      </c>
+      <c r="J855" t="s">
+        <v>12</v>
+      </c>
+      <c r="K855" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="856" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A856">
+        <v>54</v>
+      </c>
+      <c r="B856">
+        <v>1804</v>
+      </c>
+      <c r="C856" t="s">
+        <v>880</v>
+      </c>
+      <c r="F856" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H856" t="s">
+        <v>11</v>
+      </c>
+      <c r="I856">
+        <v>47</v>
+      </c>
+      <c r="J856" t="s">
+        <v>12</v>
+      </c>
+      <c r="K856" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="857" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A857">
+        <v>54</v>
+      </c>
+      <c r="B857">
+        <v>1804</v>
+      </c>
+      <c r="C857" t="s">
+        <v>881</v>
+      </c>
+      <c r="F857" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H857" t="s">
+        <v>11</v>
+      </c>
+      <c r="I857">
+        <v>47</v>
+      </c>
+      <c r="J857" t="s">
+        <v>12</v>
+      </c>
+      <c r="K857" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="858" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A858">
+        <v>54</v>
+      </c>
+      <c r="B858">
+        <v>1804</v>
+      </c>
+      <c r="C858" t="s">
+        <v>882</v>
+      </c>
+      <c r="F858" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H858" t="s">
+        <v>11</v>
+      </c>
+      <c r="I858">
+        <v>47</v>
+      </c>
+      <c r="J858" t="s">
+        <v>12</v>
+      </c>
+      <c r="K858" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="859" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A859">
+        <v>54</v>
+      </c>
+      <c r="B859">
+        <v>1804</v>
+      </c>
+      <c r="C859" t="s">
+        <v>883</v>
+      </c>
+      <c r="F859" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H859" t="s">
+        <v>11</v>
+      </c>
+      <c r="I859">
+        <v>47</v>
+      </c>
+      <c r="J859" t="s">
+        <v>12</v>
+      </c>
+      <c r="K859" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="860" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A860">
+        <v>54</v>
+      </c>
+      <c r="B860">
+        <v>1804</v>
+      </c>
+      <c r="C860" t="s">
+        <v>884</v>
+      </c>
+      <c r="F860" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H860" t="s">
+        <v>11</v>
+      </c>
+      <c r="I860">
+        <v>47</v>
+      </c>
+      <c r="J860" t="s">
+        <v>12</v>
+      </c>
+      <c r="K860" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="861" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A861">
+        <v>54</v>
+      </c>
+      <c r="B861">
+        <v>1804</v>
+      </c>
+      <c r="C861" t="s">
+        <v>885</v>
+      </c>
+      <c r="F861" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H861" t="s">
+        <v>11</v>
+      </c>
+      <c r="I861">
+        <v>47</v>
+      </c>
+      <c r="J861" t="s">
+        <v>12</v>
+      </c>
+      <c r="K861" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="862" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A862">
+        <v>54</v>
+      </c>
+      <c r="B862">
+        <v>1804</v>
+      </c>
+      <c r="C862" t="s">
+        <v>886</v>
+      </c>
+      <c r="F862" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H862" t="s">
+        <v>11</v>
+      </c>
+      <c r="I862">
+        <v>47</v>
+      </c>
+      <c r="J862" t="s">
+        <v>12</v>
+      </c>
+      <c r="K862" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="863" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A863">
+        <v>54</v>
+      </c>
+      <c r="B863">
+        <v>1804</v>
+      </c>
+      <c r="C863" t="s">
+        <v>887</v>
+      </c>
+      <c r="F863" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H863" t="s">
+        <v>11</v>
+      </c>
+      <c r="I863">
+        <v>47</v>
+      </c>
+      <c r="J863" t="s">
+        <v>12</v>
+      </c>
+      <c r="K863" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="864" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A864">
+        <v>54</v>
+      </c>
+      <c r="B864">
+        <v>1804</v>
+      </c>
+      <c r="C864" t="s">
+        <v>888</v>
+      </c>
+      <c r="F864" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H864" t="s">
+        <v>11</v>
+      </c>
+      <c r="I864">
+        <v>47</v>
+      </c>
+      <c r="J864" t="s">
+        <v>12</v>
+      </c>
+      <c r="K864" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="865" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A865">
+        <v>54</v>
+      </c>
+      <c r="B865">
+        <v>1804</v>
+      </c>
+      <c r="C865" t="s">
+        <v>889</v>
+      </c>
+      <c r="F865" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H865" t="s">
+        <v>11</v>
+      </c>
+      <c r="I865">
+        <v>47</v>
+      </c>
+      <c r="J865" t="s">
+        <v>12</v>
+      </c>
+      <c r="K865" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="866" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A866">
+        <v>54</v>
+      </c>
+      <c r="B866">
+        <v>1804</v>
+      </c>
+      <c r="C866" t="s">
+        <v>890</v>
+      </c>
+      <c r="F866" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H866" t="s">
+        <v>11</v>
+      </c>
+      <c r="I866">
+        <v>47</v>
+      </c>
+      <c r="J866" t="s">
+        <v>12</v>
+      </c>
+      <c r="K866" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="867" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A867">
+        <v>54</v>
+      </c>
+      <c r="B867">
+        <v>1804</v>
+      </c>
+      <c r="C867" t="s">
+        <v>891</v>
+      </c>
+      <c r="F867" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H867" t="s">
+        <v>11</v>
+      </c>
+      <c r="I867">
+        <v>47</v>
+      </c>
+      <c r="J867" t="s">
+        <v>12</v>
+      </c>
+      <c r="K867" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="868" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A868">
+        <v>54</v>
+      </c>
+      <c r="B868">
+        <v>1804</v>
+      </c>
+      <c r="C868" t="s">
+        <v>892</v>
+      </c>
+      <c r="F868" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H868" t="s">
+        <v>11</v>
+      </c>
+      <c r="I868">
+        <v>47</v>
+      </c>
+      <c r="J868" t="s">
+        <v>12</v>
+      </c>
+      <c r="K868" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="869" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A869">
+        <v>54</v>
+      </c>
+      <c r="B869">
+        <v>1804</v>
+      </c>
+      <c r="C869" t="s">
+        <v>893</v>
+      </c>
+      <c r="F869" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H869" t="s">
+        <v>11</v>
+      </c>
+      <c r="I869">
+        <v>47</v>
+      </c>
+      <c r="J869" t="s">
+        <v>12</v>
+      </c>
+      <c r="K869" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="870" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A870">
+        <v>54</v>
+      </c>
+      <c r="B870">
+        <v>1804</v>
+      </c>
+      <c r="C870" t="s">
+        <v>894</v>
+      </c>
+      <c r="F870" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H870" t="s">
+        <v>11</v>
+      </c>
+      <c r="I870">
+        <v>47</v>
+      </c>
+      <c r="J870" t="s">
+        <v>12</v>
+      </c>
+      <c r="K870" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="871" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A871">
+        <v>54</v>
+      </c>
+      <c r="B871">
+        <v>1804</v>
+      </c>
+      <c r="C871" t="s">
+        <v>895</v>
+      </c>
+      <c r="F871" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H871" t="s">
+        <v>11</v>
+      </c>
+      <c r="I871">
+        <v>47</v>
+      </c>
+      <c r="J871" t="s">
+        <v>12</v>
+      </c>
+      <c r="K871" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="872" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A872">
+        <v>54</v>
+      </c>
+      <c r="B872">
+        <v>1804</v>
+      </c>
+      <c r="C872" t="s">
+        <v>896</v>
+      </c>
+      <c r="F872" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H872" t="s">
+        <v>11</v>
+      </c>
+      <c r="I872">
+        <v>47</v>
+      </c>
+      <c r="J872" t="s">
+        <v>12</v>
+      </c>
+      <c r="K872" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="873" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A873">
+        <v>54</v>
+      </c>
+      <c r="B873">
+        <v>1804</v>
+      </c>
+      <c r="C873" t="s">
+        <v>897</v>
+      </c>
+      <c r="F873" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H873" t="s">
+        <v>11</v>
+      </c>
+      <c r="I873">
+        <v>47</v>
+      </c>
+      <c r="J873" t="s">
+        <v>12</v>
+      </c>
+      <c r="K873" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="874" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A874">
+        <v>54</v>
+      </c>
+      <c r="B874">
+        <v>1804</v>
+      </c>
+      <c r="C874" t="s">
+        <v>898</v>
+      </c>
+      <c r="F874" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H874" t="s">
+        <v>11</v>
+      </c>
+      <c r="I874">
+        <v>47</v>
+      </c>
+      <c r="J874" t="s">
+        <v>12</v>
+      </c>
+      <c r="K874" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="875" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A875">
+        <v>53</v>
+      </c>
+      <c r="B875">
+        <v>1804</v>
+      </c>
+      <c r="C875" t="s">
+        <v>899</v>
+      </c>
+      <c r="F875" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H875" t="s">
+        <v>11</v>
+      </c>
+      <c r="I875">
+        <v>47</v>
+      </c>
+      <c r="J875" t="s">
+        <v>12</v>
+      </c>
+      <c r="K875" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="876" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A876">
+        <v>53</v>
+      </c>
+      <c r="B876">
+        <v>1804</v>
+      </c>
+      <c r="C876" t="s">
+        <v>900</v>
+      </c>
+      <c r="F876" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H876" t="s">
+        <v>11</v>
+      </c>
+      <c r="I876">
+        <v>47</v>
+      </c>
+      <c r="J876" t="s">
+        <v>12</v>
+      </c>
+      <c r="K876" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="877" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A877">
+        <v>53</v>
+      </c>
+      <c r="B877">
+        <v>1804</v>
+      </c>
+      <c r="C877" t="s">
+        <v>901</v>
+      </c>
+      <c r="F877" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H877" t="s">
+        <v>11</v>
+      </c>
+      <c r="I877">
+        <v>47</v>
+      </c>
+      <c r="J877" t="s">
+        <v>12</v>
+      </c>
+      <c r="K877" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="878" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A878">
+        <v>53</v>
+      </c>
+      <c r="B878">
+        <v>1804</v>
+      </c>
+      <c r="C878" t="s">
+        <v>902</v>
+      </c>
+      <c r="F878" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H878" t="s">
+        <v>11</v>
+      </c>
+      <c r="I878">
+        <v>47</v>
+      </c>
+      <c r="J878" t="s">
+        <v>12</v>
+      </c>
+      <c r="K878" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="879" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A879">
+        <v>53</v>
+      </c>
+      <c r="B879">
+        <v>1804</v>
+      </c>
+      <c r="C879" t="s">
+        <v>903</v>
+      </c>
+      <c r="F879" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H879" t="s">
+        <v>11</v>
+      </c>
+      <c r="I879">
+        <v>47</v>
+      </c>
+      <c r="J879" t="s">
+        <v>12</v>
+      </c>
+      <c r="K879" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="880" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A880">
+        <v>53</v>
+      </c>
+      <c r="B880">
+        <v>1804</v>
+      </c>
+      <c r="C880" t="s">
+        <v>904</v>
+      </c>
+      <c r="F880" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H880" t="s">
+        <v>11</v>
+      </c>
+      <c r="I880">
+        <v>47</v>
+      </c>
+      <c r="J880" t="s">
+        <v>12</v>
+      </c>
+      <c r="K880" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="881" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A881">
+        <v>53</v>
+      </c>
+      <c r="B881">
+        <v>1804</v>
+      </c>
+      <c r="C881" t="s">
+        <v>905</v>
+      </c>
+      <c r="F881" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H881" t="s">
+        <v>11</v>
+      </c>
+      <c r="I881">
+        <v>47</v>
+      </c>
+      <c r="J881" t="s">
+        <v>12</v>
+      </c>
+      <c r="K881" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="882" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A882">
+        <v>53</v>
+      </c>
+      <c r="B882">
+        <v>1804</v>
+      </c>
+      <c r="C882" t="s">
+        <v>906</v>
+      </c>
+      <c r="F882" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H882" t="s">
+        <v>11</v>
+      </c>
+      <c r="I882">
+        <v>47</v>
+      </c>
+      <c r="J882" t="s">
+        <v>12</v>
+      </c>
+      <c r="K882" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="883" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A883">
+        <v>53</v>
+      </c>
+      <c r="B883">
+        <v>1804</v>
+      </c>
+      <c r="C883" t="s">
+        <v>907</v>
+      </c>
+      <c r="F883" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H883" t="s">
+        <v>11</v>
+      </c>
+      <c r="I883">
+        <v>47</v>
+      </c>
+      <c r="J883" t="s">
+        <v>12</v>
+      </c>
+      <c r="K883" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="884" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A884">
+        <v>53</v>
+      </c>
+      <c r="B884">
+        <v>1804</v>
+      </c>
+      <c r="C884" t="s">
+        <v>908</v>
+      </c>
+      <c r="F884" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H884" t="s">
+        <v>11</v>
+      </c>
+      <c r="I884">
+        <v>47</v>
+      </c>
+      <c r="J884" t="s">
+        <v>12</v>
+      </c>
+      <c r="K884" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="885" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A885">
+        <v>53</v>
+      </c>
+      <c r="B885">
+        <v>1804</v>
+      </c>
+      <c r="C885" t="s">
+        <v>909</v>
+      </c>
+      <c r="F885" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H885" t="s">
+        <v>11</v>
+      </c>
+      <c r="I885">
+        <v>47</v>
+      </c>
+      <c r="J885" t="s">
+        <v>12</v>
+      </c>
+      <c r="K885" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="886" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A886">
+        <v>53</v>
+      </c>
+      <c r="B886">
+        <v>1804</v>
+      </c>
+      <c r="C886" t="s">
+        <v>910</v>
+      </c>
+      <c r="F886" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H886" t="s">
+        <v>11</v>
+      </c>
+      <c r="I886">
+        <v>47</v>
+      </c>
+      <c r="J886" t="s">
+        <v>12</v>
+      </c>
+      <c r="K886" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="887" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A887">
+        <v>53</v>
+      </c>
+      <c r="B887">
+        <v>1804</v>
+      </c>
+      <c r="C887" t="s">
+        <v>911</v>
+      </c>
+      <c r="F887" s="1">
+        <v>1744</v>
+      </c>
+      <c r="H887" t="s">
+        <v>11</v>
+      </c>
+      <c r="I887">
+        <v>47</v>
+      </c>
+      <c r="J887" t="s">
+        <v>12</v>
+      </c>
+      <c r="K887" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Afegida indexació confirmacions any 1904 (corregit typo en l'any)
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Confirmacions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F3CDCE-C534-4EFE-A0BF-1893F7E08655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C609C9-5665-4B74-B2CC-A9E839FB7EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FEEAE0F-87B7-4CFD-9217-CD5D622A9875}"/>
   </bookViews>
@@ -3143,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EAC519-AAA9-4752-A1C1-63CDDDDDC53A}">
   <dimension ref="A1:L887"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A855" workbookViewId="0">
-      <selection activeCell="E883" sqref="E883"/>
+    <sheetView tabSelected="1" topLeftCell="A864" workbookViewId="0">
+      <selection activeCell="A888" sqref="A888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13946,7 +13946,7 @@
         <v>60</v>
       </c>
       <c r="B370">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C370" t="s">
         <v>395</v>
@@ -13975,7 +13975,7 @@
         <v>60</v>
       </c>
       <c r="B371">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C371" t="s">
         <v>396</v>
@@ -14004,7 +14004,7 @@
         <v>60</v>
       </c>
       <c r="B372">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C372" t="s">
         <v>397</v>
@@ -14033,7 +14033,7 @@
         <v>60</v>
       </c>
       <c r="B373">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C373" t="s">
         <v>398</v>
@@ -14062,7 +14062,7 @@
         <v>60</v>
       </c>
       <c r="B374">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C374" t="s">
         <v>399</v>
@@ -14091,7 +14091,7 @@
         <v>60</v>
       </c>
       <c r="B375">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C375" t="s">
         <v>400</v>
@@ -14120,7 +14120,7 @@
         <v>60</v>
       </c>
       <c r="B376">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C376" t="s">
         <v>401</v>
@@ -14149,7 +14149,7 @@
         <v>60</v>
       </c>
       <c r="B377">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C377" t="s">
         <v>402</v>
@@ -14178,7 +14178,7 @@
         <v>60</v>
       </c>
       <c r="B378">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C378" t="s">
         <v>403</v>
@@ -14207,7 +14207,7 @@
         <v>60</v>
       </c>
       <c r="B379">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C379" t="s">
         <v>404</v>
@@ -14236,7 +14236,7 @@
         <v>60</v>
       </c>
       <c r="B380">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C380" t="s">
         <v>405</v>
@@ -14265,7 +14265,7 @@
         <v>60</v>
       </c>
       <c r="B381">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C381" t="s">
         <v>406</v>
@@ -14294,7 +14294,7 @@
         <v>60</v>
       </c>
       <c r="B382">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C382" t="s">
         <v>407</v>
@@ -14323,7 +14323,7 @@
         <v>60</v>
       </c>
       <c r="B383">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C383" t="s">
         <v>408</v>
@@ -14352,7 +14352,7 @@
         <v>60</v>
       </c>
       <c r="B384">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C384" t="s">
         <v>409</v>
@@ -14381,7 +14381,7 @@
         <v>60</v>
       </c>
       <c r="B385">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C385" t="s">
         <v>410</v>
@@ -14410,7 +14410,7 @@
         <v>60</v>
       </c>
       <c r="B386">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C386" t="s">
         <v>411</v>
@@ -14439,7 +14439,7 @@
         <v>60</v>
       </c>
       <c r="B387">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C387" t="s">
         <v>412</v>
@@ -14468,7 +14468,7 @@
         <v>60</v>
       </c>
       <c r="B388">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C388" t="s">
         <v>413</v>
@@ -14497,7 +14497,7 @@
         <v>60</v>
       </c>
       <c r="B389">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C389" t="s">
         <v>414</v>
@@ -14526,7 +14526,7 @@
         <v>60</v>
       </c>
       <c r="B390">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C390" t="s">
         <v>415</v>
@@ -14555,7 +14555,7 @@
         <v>60</v>
       </c>
       <c r="B391">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C391" t="s">
         <v>416</v>
@@ -14584,7 +14584,7 @@
         <v>60</v>
       </c>
       <c r="B392">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C392" t="s">
         <v>417</v>
@@ -14613,7 +14613,7 @@
         <v>60</v>
       </c>
       <c r="B393">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C393" t="s">
         <v>418</v>
@@ -14642,7 +14642,7 @@
         <v>60</v>
       </c>
       <c r="B394">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C394" t="s">
         <v>419</v>
@@ -14671,7 +14671,7 @@
         <v>60</v>
       </c>
       <c r="B395">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C395" t="s">
         <v>420</v>
@@ -14700,7 +14700,7 @@
         <v>60</v>
       </c>
       <c r="B396">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C396" t="s">
         <v>421</v>
@@ -14729,7 +14729,7 @@
         <v>59</v>
       </c>
       <c r="B397">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C397" t="s">
         <v>422</v>
@@ -14758,7 +14758,7 @@
         <v>59</v>
       </c>
       <c r="B398">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C398" t="s">
         <v>423</v>
@@ -14787,7 +14787,7 @@
         <v>59</v>
       </c>
       <c r="B399">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C399" t="s">
         <v>424</v>
@@ -14816,7 +14816,7 @@
         <v>59</v>
       </c>
       <c r="B400">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C400" t="s">
         <v>425</v>
@@ -14845,7 +14845,7 @@
         <v>59</v>
       </c>
       <c r="B401">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C401" t="s">
         <v>426</v>
@@ -14874,7 +14874,7 @@
         <v>59</v>
       </c>
       <c r="B402">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C402" t="s">
         <v>427</v>
@@ -14903,7 +14903,7 @@
         <v>59</v>
       </c>
       <c r="B403">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C403" t="s">
         <v>428</v>
@@ -14932,7 +14932,7 @@
         <v>59</v>
       </c>
       <c r="B404">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C404" t="s">
         <v>429</v>
@@ -14961,7 +14961,7 @@
         <v>59</v>
       </c>
       <c r="B405">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C405" t="s">
         <v>430</v>
@@ -14990,7 +14990,7 @@
         <v>59</v>
       </c>
       <c r="B406">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C406" t="s">
         <v>431</v>
@@ -15019,7 +15019,7 @@
         <v>59</v>
       </c>
       <c r="B407">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C407" t="s">
         <v>432</v>
@@ -15048,7 +15048,7 @@
         <v>59</v>
       </c>
       <c r="B408">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C408" t="s">
         <v>433</v>
@@ -15077,7 +15077,7 @@
         <v>59</v>
       </c>
       <c r="B409">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C409" t="s">
         <v>434</v>
@@ -15106,7 +15106,7 @@
         <v>59</v>
       </c>
       <c r="B410">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C410" t="s">
         <v>435</v>
@@ -15135,7 +15135,7 @@
         <v>59</v>
       </c>
       <c r="B411">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C411" t="s">
         <v>436</v>
@@ -15164,7 +15164,7 @@
         <v>59</v>
       </c>
       <c r="B412">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C412" t="s">
         <v>437</v>
@@ -15193,7 +15193,7 @@
         <v>59</v>
       </c>
       <c r="B413">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C413" t="s">
         <v>438</v>
@@ -15222,7 +15222,7 @@
         <v>59</v>
       </c>
       <c r="B414">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C414" t="s">
         <v>439</v>
@@ -15251,7 +15251,7 @@
         <v>59</v>
       </c>
       <c r="B415">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C415" t="s">
         <v>440</v>
@@ -15280,7 +15280,7 @@
         <v>59</v>
       </c>
       <c r="B416">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C416" t="s">
         <v>441</v>
@@ -15309,7 +15309,7 @@
         <v>59</v>
       </c>
       <c r="B417">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C417" t="s">
         <v>442</v>
@@ -15338,7 +15338,7 @@
         <v>59</v>
       </c>
       <c r="B418">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C418" t="s">
         <v>443</v>
@@ -15367,7 +15367,7 @@
         <v>59</v>
       </c>
       <c r="B419">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C419" t="s">
         <v>444</v>
@@ -15396,7 +15396,7 @@
         <v>59</v>
       </c>
       <c r="B420">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C420" t="s">
         <v>445</v>
@@ -15425,7 +15425,7 @@
         <v>59</v>
       </c>
       <c r="B421">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C421" t="s">
         <v>446</v>
@@ -15454,7 +15454,7 @@
         <v>59</v>
       </c>
       <c r="B422">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C422" t="s">
         <v>447</v>
@@ -15483,7 +15483,7 @@
         <v>59</v>
       </c>
       <c r="B423">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C423" t="s">
         <v>448</v>
@@ -15512,7 +15512,7 @@
         <v>59</v>
       </c>
       <c r="B424">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C424" t="s">
         <v>449</v>
@@ -15541,7 +15541,7 @@
         <v>59</v>
       </c>
       <c r="B425">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C425" t="s">
         <v>450</v>
@@ -15570,7 +15570,7 @@
         <v>59</v>
       </c>
       <c r="B426">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C426" t="s">
         <v>451</v>
@@ -15599,7 +15599,7 @@
         <v>59</v>
       </c>
       <c r="B427">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C427" t="s">
         <v>452</v>
@@ -15628,7 +15628,7 @@
         <v>59</v>
       </c>
       <c r="B428">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C428" t="s">
         <v>453</v>
@@ -15657,7 +15657,7 @@
         <v>59</v>
       </c>
       <c r="B429">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C429" t="s">
         <v>454</v>
@@ -15686,7 +15686,7 @@
         <v>59</v>
       </c>
       <c r="B430">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C430" t="s">
         <v>455</v>
@@ -15715,7 +15715,7 @@
         <v>59</v>
       </c>
       <c r="B431">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C431" t="s">
         <v>456</v>
@@ -15744,7 +15744,7 @@
         <v>59</v>
       </c>
       <c r="B432">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C432" t="s">
         <v>457</v>
@@ -15773,7 +15773,7 @@
         <v>59</v>
       </c>
       <c r="B433">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C433" t="s">
         <v>458</v>
@@ -15802,7 +15802,7 @@
         <v>59</v>
       </c>
       <c r="B434">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C434" t="s">
         <v>459</v>
@@ -15831,7 +15831,7 @@
         <v>59</v>
       </c>
       <c r="B435">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C435" t="s">
         <v>460</v>
@@ -15860,7 +15860,7 @@
         <v>59</v>
       </c>
       <c r="B436">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C436" t="s">
         <v>461</v>
@@ -15889,7 +15889,7 @@
         <v>59</v>
       </c>
       <c r="B437">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C437" t="s">
         <v>462</v>
@@ -15918,7 +15918,7 @@
         <v>59</v>
       </c>
       <c r="B438">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C438" t="s">
         <v>463</v>
@@ -15947,7 +15947,7 @@
         <v>59</v>
       </c>
       <c r="B439">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C439" t="s">
         <v>464</v>
@@ -15976,7 +15976,7 @@
         <v>59</v>
       </c>
       <c r="B440">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C440" t="s">
         <v>465</v>
@@ -16005,7 +16005,7 @@
         <v>59</v>
       </c>
       <c r="B441">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C441" t="s">
         <v>466</v>
@@ -16034,7 +16034,7 @@
         <v>59</v>
       </c>
       <c r="B442">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C442" t="s">
         <v>467</v>
@@ -16063,7 +16063,7 @@
         <v>59</v>
       </c>
       <c r="B443">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C443" t="s">
         <v>468</v>
@@ -16092,7 +16092,7 @@
         <v>59</v>
       </c>
       <c r="B444">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C444" t="s">
         <v>469</v>
@@ -16121,7 +16121,7 @@
         <v>59</v>
       </c>
       <c r="B445">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C445" t="s">
         <v>470</v>
@@ -16150,7 +16150,7 @@
         <v>59</v>
       </c>
       <c r="B446">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C446" t="s">
         <v>471</v>
@@ -16179,7 +16179,7 @@
         <v>59</v>
       </c>
       <c r="B447">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C447" t="s">
         <v>472</v>
@@ -16208,7 +16208,7 @@
         <v>59</v>
       </c>
       <c r="B448">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C448" t="s">
         <v>473</v>
@@ -16237,7 +16237,7 @@
         <v>59</v>
       </c>
       <c r="B449">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C449" t="s">
         <v>474</v>
@@ -16266,7 +16266,7 @@
         <v>59</v>
       </c>
       <c r="B450">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C450" t="s">
         <v>475</v>
@@ -16295,7 +16295,7 @@
         <v>59</v>
       </c>
       <c r="B451">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C451" t="s">
         <v>476</v>
@@ -16324,7 +16324,7 @@
         <v>59</v>
       </c>
       <c r="B452">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C452" t="s">
         <v>477</v>
@@ -16353,7 +16353,7 @@
         <v>59</v>
       </c>
       <c r="B453">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C453" t="s">
         <v>478</v>
@@ -16382,7 +16382,7 @@
         <v>59</v>
       </c>
       <c r="B454">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C454" t="s">
         <v>479</v>
@@ -16411,7 +16411,7 @@
         <v>59</v>
       </c>
       <c r="B455">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C455" t="s">
         <v>480</v>
@@ -16440,7 +16440,7 @@
         <v>59</v>
       </c>
       <c r="B456">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C456" t="s">
         <v>481</v>
@@ -16469,7 +16469,7 @@
         <v>59</v>
       </c>
       <c r="B457">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C457" t="s">
         <v>482</v>
@@ -16498,7 +16498,7 @@
         <v>59</v>
       </c>
       <c r="B458">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C458" t="s">
         <v>483</v>
@@ -16527,7 +16527,7 @@
         <v>59</v>
       </c>
       <c r="B459">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C459" t="s">
         <v>484</v>
@@ -16556,7 +16556,7 @@
         <v>59</v>
       </c>
       <c r="B460">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C460" t="s">
         <v>485</v>
@@ -16585,7 +16585,7 @@
         <v>59</v>
       </c>
       <c r="B461">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C461" t="s">
         <v>486</v>
@@ -16614,7 +16614,7 @@
         <v>59</v>
       </c>
       <c r="B462">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C462" t="s">
         <v>487</v>
@@ -16643,7 +16643,7 @@
         <v>59</v>
       </c>
       <c r="B463">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C463" t="s">
         <v>488</v>
@@ -16672,7 +16672,7 @@
         <v>59</v>
       </c>
       <c r="B464">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C464" t="s">
         <v>489</v>
@@ -16701,7 +16701,7 @@
         <v>59</v>
       </c>
       <c r="B465">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C465" t="s">
         <v>490</v>
@@ -16730,7 +16730,7 @@
         <v>59</v>
       </c>
       <c r="B466">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C466" t="s">
         <v>491</v>
@@ -16759,7 +16759,7 @@
         <v>59</v>
       </c>
       <c r="B467">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C467" t="s">
         <v>492</v>
@@ -16788,7 +16788,7 @@
         <v>59</v>
       </c>
       <c r="B468">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C468" t="s">
         <v>493</v>
@@ -16817,7 +16817,7 @@
         <v>59</v>
       </c>
       <c r="B469">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C469" t="s">
         <v>494</v>
@@ -16846,7 +16846,7 @@
         <v>59</v>
       </c>
       <c r="B470">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C470" t="s">
         <v>495</v>
@@ -16875,7 +16875,7 @@
         <v>59</v>
       </c>
       <c r="B471">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C471" t="s">
         <v>496</v>
@@ -16904,7 +16904,7 @@
         <v>59</v>
       </c>
       <c r="B472">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C472" t="s">
         <v>497</v>
@@ -16933,7 +16933,7 @@
         <v>59</v>
       </c>
       <c r="B473">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C473" t="s">
         <v>498</v>
@@ -16962,7 +16962,7 @@
         <v>59</v>
       </c>
       <c r="B474">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C474" t="s">
         <v>499</v>
@@ -16991,7 +16991,7 @@
         <v>59</v>
       </c>
       <c r="B475">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C475" t="s">
         <v>500</v>
@@ -17020,7 +17020,7 @@
         <v>58</v>
       </c>
       <c r="B476">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C476" t="s">
         <v>504</v>
@@ -17049,7 +17049,7 @@
         <v>58</v>
       </c>
       <c r="B477">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C477" t="s">
         <v>505</v>
@@ -17078,7 +17078,7 @@
         <v>58</v>
       </c>
       <c r="B478">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C478" t="s">
         <v>506</v>
@@ -17107,7 +17107,7 @@
         <v>58</v>
       </c>
       <c r="B479">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C479" t="s">
         <v>507</v>
@@ -17136,7 +17136,7 @@
         <v>58</v>
       </c>
       <c r="B480">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C480" t="s">
         <v>508</v>
@@ -17165,7 +17165,7 @@
         <v>58</v>
       </c>
       <c r="B481">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C481" t="s">
         <v>509</v>
@@ -17194,7 +17194,7 @@
         <v>58</v>
       </c>
       <c r="B482">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C482" t="s">
         <v>510</v>
@@ -17223,7 +17223,7 @@
         <v>58</v>
       </c>
       <c r="B483">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C483" t="s">
         <v>511</v>
@@ -17252,7 +17252,7 @@
         <v>58</v>
       </c>
       <c r="B484">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C484" t="s">
         <v>512</v>
@@ -17281,7 +17281,7 @@
         <v>58</v>
       </c>
       <c r="B485">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C485" t="s">
         <v>513</v>
@@ -17310,7 +17310,7 @@
         <v>58</v>
       </c>
       <c r="B486">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C486" t="s">
         <v>514</v>
@@ -17339,7 +17339,7 @@
         <v>58</v>
       </c>
       <c r="B487">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C487" t="s">
         <v>515</v>
@@ -17368,7 +17368,7 @@
         <v>58</v>
       </c>
       <c r="B488">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C488" t="s">
         <v>516</v>
@@ -17397,7 +17397,7 @@
         <v>58</v>
       </c>
       <c r="B489">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C489" t="s">
         <v>517</v>
@@ -17426,7 +17426,7 @@
         <v>58</v>
       </c>
       <c r="B490">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C490" t="s">
         <v>518</v>
@@ -17455,7 +17455,7 @@
         <v>58</v>
       </c>
       <c r="B491">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C491" t="s">
         <v>519</v>
@@ -17484,7 +17484,7 @@
         <v>58</v>
       </c>
       <c r="B492">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C492" t="s">
         <v>520</v>
@@ -17513,7 +17513,7 @@
         <v>58</v>
       </c>
       <c r="B493">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C493" t="s">
         <v>521</v>
@@ -17542,7 +17542,7 @@
         <v>58</v>
       </c>
       <c r="B494">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C494" t="s">
         <v>522</v>
@@ -17571,7 +17571,7 @@
         <v>58</v>
       </c>
       <c r="B495">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C495" t="s">
         <v>523</v>
@@ -17600,7 +17600,7 @@
         <v>58</v>
       </c>
       <c r="B496">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C496" t="s">
         <v>524</v>
@@ -17629,7 +17629,7 @@
         <v>58</v>
       </c>
       <c r="B497">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C497" t="s">
         <v>525</v>
@@ -17658,7 +17658,7 @@
         <v>58</v>
       </c>
       <c r="B498">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C498" t="s">
         <v>526</v>
@@ -17687,7 +17687,7 @@
         <v>58</v>
       </c>
       <c r="B499">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C499" t="s">
         <v>527</v>
@@ -17716,7 +17716,7 @@
         <v>58</v>
       </c>
       <c r="B500">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C500" t="s">
         <v>528</v>
@@ -17745,7 +17745,7 @@
         <v>58</v>
       </c>
       <c r="B501">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C501" t="s">
         <v>529</v>
@@ -17774,7 +17774,7 @@
         <v>58</v>
       </c>
       <c r="B502">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C502" t="s">
         <v>347</v>
@@ -17803,7 +17803,7 @@
         <v>58</v>
       </c>
       <c r="B503">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C503" t="s">
         <v>530</v>
@@ -17832,7 +17832,7 @@
         <v>58</v>
       </c>
       <c r="B504">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C504" t="s">
         <v>531</v>
@@ -17861,7 +17861,7 @@
         <v>58</v>
       </c>
       <c r="B505">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C505" t="s">
         <v>532</v>
@@ -17890,7 +17890,7 @@
         <v>58</v>
       </c>
       <c r="B506">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C506" t="s">
         <v>533</v>
@@ -17919,7 +17919,7 @@
         <v>58</v>
       </c>
       <c r="B507">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C507" t="s">
         <v>534</v>
@@ -17948,7 +17948,7 @@
         <v>58</v>
       </c>
       <c r="B508">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C508" t="s">
         <v>535</v>
@@ -17977,7 +17977,7 @@
         <v>58</v>
       </c>
       <c r="B509">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C509" t="s">
         <v>536</v>
@@ -18006,7 +18006,7 @@
         <v>58</v>
       </c>
       <c r="B510">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C510" t="s">
         <v>537</v>
@@ -18035,7 +18035,7 @@
         <v>58</v>
       </c>
       <c r="B511">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C511" t="s">
         <v>538</v>
@@ -18064,7 +18064,7 @@
         <v>58</v>
       </c>
       <c r="B512">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C512" t="s">
         <v>539</v>
@@ -18093,7 +18093,7 @@
         <v>58</v>
       </c>
       <c r="B513">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C513" t="s">
         <v>540</v>
@@ -18122,7 +18122,7 @@
         <v>58</v>
       </c>
       <c r="B514">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C514" t="s">
         <v>541</v>
@@ -18151,7 +18151,7 @@
         <v>58</v>
       </c>
       <c r="B515">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C515" t="s">
         <v>542</v>
@@ -18180,7 +18180,7 @@
         <v>58</v>
       </c>
       <c r="B516">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C516" t="s">
         <v>543</v>
@@ -18209,7 +18209,7 @@
         <v>58</v>
       </c>
       <c r="B517">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C517" t="s">
         <v>544</v>
@@ -18238,7 +18238,7 @@
         <v>58</v>
       </c>
       <c r="B518">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C518" t="s">
         <v>545</v>
@@ -18267,7 +18267,7 @@
         <v>58</v>
       </c>
       <c r="B519">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C519" t="s">
         <v>546</v>
@@ -18296,7 +18296,7 @@
         <v>58</v>
       </c>
       <c r="B520">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C520" t="s">
         <v>547</v>
@@ -18325,7 +18325,7 @@
         <v>58</v>
       </c>
       <c r="B521">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C521" t="s">
         <v>548</v>
@@ -18354,7 +18354,7 @@
         <v>58</v>
       </c>
       <c r="B522">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C522" t="s">
         <v>549</v>
@@ -18383,7 +18383,7 @@
         <v>58</v>
       </c>
       <c r="B523">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C523" t="s">
         <v>550</v>
@@ -18412,7 +18412,7 @@
         <v>58</v>
       </c>
       <c r="B524">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C524" t="s">
         <v>551</v>
@@ -18441,7 +18441,7 @@
         <v>58</v>
       </c>
       <c r="B525">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C525" t="s">
         <v>552</v>
@@ -18470,7 +18470,7 @@
         <v>58</v>
       </c>
       <c r="B526">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C526" t="s">
         <v>553</v>
@@ -18499,7 +18499,7 @@
         <v>58</v>
       </c>
       <c r="B527">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C527" t="s">
         <v>554</v>
@@ -18528,7 +18528,7 @@
         <v>58</v>
       </c>
       <c r="B528">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C528" t="s">
         <v>555</v>
@@ -18557,7 +18557,7 @@
         <v>58</v>
       </c>
       <c r="B529">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C529" t="s">
         <v>556</v>
@@ -18586,7 +18586,7 @@
         <v>58</v>
       </c>
       <c r="B530">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C530" t="s">
         <v>557</v>
@@ -18615,7 +18615,7 @@
         <v>58</v>
       </c>
       <c r="B531">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C531" t="s">
         <v>558</v>
@@ -18644,7 +18644,7 @@
         <v>58</v>
       </c>
       <c r="B532">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C532" t="s">
         <v>559</v>
@@ -18673,7 +18673,7 @@
         <v>58</v>
       </c>
       <c r="B533">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C533" t="s">
         <v>560</v>
@@ -18702,7 +18702,7 @@
         <v>58</v>
       </c>
       <c r="B534">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C534" t="s">
         <v>561</v>
@@ -18731,7 +18731,7 @@
         <v>58</v>
       </c>
       <c r="B535">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C535" t="s">
         <v>562</v>
@@ -18760,7 +18760,7 @@
         <v>58</v>
       </c>
       <c r="B536">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C536" t="s">
         <v>563</v>
@@ -18789,7 +18789,7 @@
         <v>58</v>
       </c>
       <c r="B537">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C537" t="s">
         <v>564</v>
@@ -18818,7 +18818,7 @@
         <v>58</v>
       </c>
       <c r="B538">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C538" t="s">
         <v>565</v>
@@ -18847,7 +18847,7 @@
         <v>58</v>
       </c>
       <c r="B539">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C539" t="s">
         <v>566</v>
@@ -18876,7 +18876,7 @@
         <v>58</v>
       </c>
       <c r="B540">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C540" t="s">
         <v>567</v>
@@ -18905,7 +18905,7 @@
         <v>58</v>
       </c>
       <c r="B541">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C541" t="s">
         <v>568</v>
@@ -18934,7 +18934,7 @@
         <v>58</v>
       </c>
       <c r="B542">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C542" t="s">
         <v>569</v>
@@ -18963,7 +18963,7 @@
         <v>58</v>
       </c>
       <c r="B543">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C543" t="s">
         <v>570</v>
@@ -18992,7 +18992,7 @@
         <v>58</v>
       </c>
       <c r="B544">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C544" t="s">
         <v>571</v>
@@ -19021,7 +19021,7 @@
         <v>58</v>
       </c>
       <c r="B545">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C545" t="s">
         <v>572</v>
@@ -19050,7 +19050,7 @@
         <v>58</v>
       </c>
       <c r="B546">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C546" t="s">
         <v>573</v>
@@ -19079,7 +19079,7 @@
         <v>58</v>
       </c>
       <c r="B547">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C547" t="s">
         <v>574</v>
@@ -19108,7 +19108,7 @@
         <v>58</v>
       </c>
       <c r="B548">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C548" t="s">
         <v>575</v>
@@ -19137,7 +19137,7 @@
         <v>58</v>
       </c>
       <c r="B549">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C549" t="s">
         <v>576</v>
@@ -19166,7 +19166,7 @@
         <v>58</v>
       </c>
       <c r="B550">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C550" t="s">
         <v>577</v>
@@ -19195,7 +19195,7 @@
         <v>58</v>
       </c>
       <c r="B551">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C551" t="s">
         <v>578</v>
@@ -19224,7 +19224,7 @@
         <v>58</v>
       </c>
       <c r="B552">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C552" t="s">
         <v>579</v>
@@ -19253,7 +19253,7 @@
         <v>58</v>
       </c>
       <c r="B553">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C553" t="s">
         <v>580</v>
@@ -19282,7 +19282,7 @@
         <v>58</v>
       </c>
       <c r="B554">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C554" t="s">
         <v>581</v>
@@ -19311,7 +19311,7 @@
         <v>58</v>
       </c>
       <c r="B555">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C555" t="s">
         <v>582</v>
@@ -19340,7 +19340,7 @@
         <v>58</v>
       </c>
       <c r="B556">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C556" t="s">
         <v>583</v>
@@ -19369,7 +19369,7 @@
         <v>57</v>
       </c>
       <c r="B557">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C557" t="s">
         <v>585</v>
@@ -19395,7 +19395,7 @@
         <v>57</v>
       </c>
       <c r="B558">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C558" t="s">
         <v>584</v>
@@ -19421,7 +19421,7 @@
         <v>57</v>
       </c>
       <c r="B559">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C559" t="s">
         <v>586</v>
@@ -19447,7 +19447,7 @@
         <v>57</v>
       </c>
       <c r="B560">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C560" t="s">
         <v>587</v>
@@ -19473,7 +19473,7 @@
         <v>57</v>
       </c>
       <c r="B561">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C561" t="s">
         <v>588</v>
@@ -19499,7 +19499,7 @@
         <v>57</v>
       </c>
       <c r="B562">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C562" t="s">
         <v>589</v>
@@ -19525,7 +19525,7 @@
         <v>57</v>
       </c>
       <c r="B563">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C563" t="s">
         <v>590</v>
@@ -19551,7 +19551,7 @@
         <v>57</v>
       </c>
       <c r="B564">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C564" t="s">
         <v>591</v>
@@ -19577,7 +19577,7 @@
         <v>57</v>
       </c>
       <c r="B565">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C565" t="s">
         <v>592</v>
@@ -19603,7 +19603,7 @@
         <v>57</v>
       </c>
       <c r="B566">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C566" t="s">
         <v>593</v>
@@ -19629,7 +19629,7 @@
         <v>57</v>
       </c>
       <c r="B567">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C567" t="s">
         <v>594</v>
@@ -19655,7 +19655,7 @@
         <v>57</v>
       </c>
       <c r="B568">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C568" t="s">
         <v>595</v>
@@ -19681,7 +19681,7 @@
         <v>57</v>
       </c>
       <c r="B569">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C569" t="s">
         <v>596</v>
@@ -19707,7 +19707,7 @@
         <v>57</v>
       </c>
       <c r="B570">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C570" t="s">
         <v>597</v>
@@ -19733,7 +19733,7 @@
         <v>57</v>
       </c>
       <c r="B571">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C571" t="s">
         <v>598</v>
@@ -19759,7 +19759,7 @@
         <v>57</v>
       </c>
       <c r="B572">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C572" t="s">
         <v>599</v>
@@ -19785,7 +19785,7 @@
         <v>57</v>
       </c>
       <c r="B573">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C573" t="s">
         <v>600</v>
@@ -19811,7 +19811,7 @@
         <v>57</v>
       </c>
       <c r="B574">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C574" t="s">
         <v>601</v>
@@ -19837,7 +19837,7 @@
         <v>57</v>
       </c>
       <c r="B575">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C575" t="s">
         <v>602</v>
@@ -19863,7 +19863,7 @@
         <v>57</v>
       </c>
       <c r="B576">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C576" t="s">
         <v>603</v>
@@ -19889,7 +19889,7 @@
         <v>57</v>
       </c>
       <c r="B577">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C577" t="s">
         <v>508</v>
@@ -19915,7 +19915,7 @@
         <v>57</v>
       </c>
       <c r="B578">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C578" t="s">
         <v>604</v>
@@ -19941,7 +19941,7 @@
         <v>57</v>
       </c>
       <c r="B579">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C579" t="s">
         <v>605</v>
@@ -19967,7 +19967,7 @@
         <v>57</v>
       </c>
       <c r="B580">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C580" t="s">
         <v>606</v>
@@ -19993,7 +19993,7 @@
         <v>57</v>
       </c>
       <c r="B581">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C581" t="s">
         <v>607</v>
@@ -20019,7 +20019,7 @@
         <v>57</v>
       </c>
       <c r="B582">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C582" t="s">
         <v>608</v>
@@ -20045,7 +20045,7 @@
         <v>57</v>
       </c>
       <c r="B583">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C583" t="s">
         <v>609</v>
@@ -20071,7 +20071,7 @@
         <v>57</v>
       </c>
       <c r="B584">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C584" t="s">
         <v>610</v>
@@ -20097,7 +20097,7 @@
         <v>57</v>
       </c>
       <c r="B585">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C585" t="s">
         <v>611</v>
@@ -20123,7 +20123,7 @@
         <v>57</v>
       </c>
       <c r="B586">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C586" t="s">
         <v>612</v>
@@ -20149,7 +20149,7 @@
         <v>57</v>
       </c>
       <c r="B587">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C587" t="s">
         <v>613</v>
@@ -20175,7 +20175,7 @@
         <v>57</v>
       </c>
       <c r="B588">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C588" t="s">
         <v>614</v>
@@ -20201,7 +20201,7 @@
         <v>57</v>
       </c>
       <c r="B589">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C589" t="s">
         <v>615</v>
@@ -20227,7 +20227,7 @@
         <v>57</v>
       </c>
       <c r="B590">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C590" t="s">
         <v>616</v>
@@ -20253,7 +20253,7 @@
         <v>57</v>
       </c>
       <c r="B591">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C591" t="s">
         <v>617</v>
@@ -20279,7 +20279,7 @@
         <v>57</v>
       </c>
       <c r="B592">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C592" t="s">
         <v>618</v>
@@ -20305,7 +20305,7 @@
         <v>57</v>
       </c>
       <c r="B593">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C593" t="s">
         <v>619</v>
@@ -20331,7 +20331,7 @@
         <v>57</v>
       </c>
       <c r="B594">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C594" t="s">
         <v>620</v>
@@ -20357,7 +20357,7 @@
         <v>57</v>
       </c>
       <c r="B595">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C595" t="s">
         <v>621</v>
@@ -20383,7 +20383,7 @@
         <v>57</v>
       </c>
       <c r="B596">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C596" t="s">
         <v>622</v>
@@ -20409,7 +20409,7 @@
         <v>57</v>
       </c>
       <c r="B597">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C597" t="s">
         <v>623</v>
@@ -20435,7 +20435,7 @@
         <v>57</v>
       </c>
       <c r="B598">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C598" t="s">
         <v>624</v>
@@ -20461,7 +20461,7 @@
         <v>57</v>
       </c>
       <c r="B599">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C599" t="s">
         <v>625</v>
@@ -20487,7 +20487,7 @@
         <v>57</v>
       </c>
       <c r="B600">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C600" t="s">
         <v>626</v>
@@ -20513,7 +20513,7 @@
         <v>57</v>
       </c>
       <c r="B601">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C601" t="s">
         <v>627</v>
@@ -20539,7 +20539,7 @@
         <v>57</v>
       </c>
       <c r="B602">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C602" t="s">
         <v>628</v>
@@ -20565,7 +20565,7 @@
         <v>57</v>
       </c>
       <c r="B603">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C603" t="s">
         <v>629</v>
@@ -20591,7 +20591,7 @@
         <v>57</v>
       </c>
       <c r="B604">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C604" t="s">
         <v>630</v>
@@ -20617,7 +20617,7 @@
         <v>57</v>
       </c>
       <c r="B605">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C605" t="s">
         <v>631</v>
@@ -20643,7 +20643,7 @@
         <v>57</v>
       </c>
       <c r="B606">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C606" t="s">
         <v>632</v>
@@ -20669,7 +20669,7 @@
         <v>57</v>
       </c>
       <c r="B607">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C607" t="s">
         <v>633</v>
@@ -20695,7 +20695,7 @@
         <v>57</v>
       </c>
       <c r="B608">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C608" t="s">
         <v>634</v>
@@ -20721,7 +20721,7 @@
         <v>57</v>
       </c>
       <c r="B609">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C609" t="s">
         <v>635</v>
@@ -20747,7 +20747,7 @@
         <v>57</v>
       </c>
       <c r="B610">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C610" t="s">
         <v>636</v>
@@ -20773,7 +20773,7 @@
         <v>57</v>
       </c>
       <c r="B611">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C611" t="s">
         <v>637</v>
@@ -20799,7 +20799,7 @@
         <v>57</v>
       </c>
       <c r="B612">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C612" t="s">
         <v>638</v>
@@ -20825,7 +20825,7 @@
         <v>57</v>
       </c>
       <c r="B613">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C613" t="s">
         <v>639</v>
@@ -20851,7 +20851,7 @@
         <v>57</v>
       </c>
       <c r="B614">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C614" t="s">
         <v>640</v>
@@ -20877,7 +20877,7 @@
         <v>57</v>
       </c>
       <c r="B615">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C615" t="s">
         <v>641</v>
@@ -20903,7 +20903,7 @@
         <v>57</v>
       </c>
       <c r="B616">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C616" t="s">
         <v>642</v>
@@ -20929,7 +20929,7 @@
         <v>57</v>
       </c>
       <c r="B617">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C617" t="s">
         <v>643</v>
@@ -20955,7 +20955,7 @@
         <v>57</v>
       </c>
       <c r="B618">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C618" t="s">
         <v>644</v>
@@ -20981,7 +20981,7 @@
         <v>57</v>
       </c>
       <c r="B619">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C619" t="s">
         <v>645</v>
@@ -21007,7 +21007,7 @@
         <v>57</v>
       </c>
       <c r="B620">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C620" t="s">
         <v>646</v>
@@ -21033,7 +21033,7 @@
         <v>57</v>
       </c>
       <c r="B621">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C621" t="s">
         <v>647</v>
@@ -21059,7 +21059,7 @@
         <v>57</v>
       </c>
       <c r="B622">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C622" t="s">
         <v>648</v>
@@ -21085,7 +21085,7 @@
         <v>57</v>
       </c>
       <c r="B623">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C623" t="s">
         <v>649</v>
@@ -21111,7 +21111,7 @@
         <v>57</v>
       </c>
       <c r="B624">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C624" t="s">
         <v>650</v>
@@ -21137,7 +21137,7 @@
         <v>57</v>
       </c>
       <c r="B625">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C625" t="s">
         <v>651</v>
@@ -21163,7 +21163,7 @@
         <v>57</v>
       </c>
       <c r="B626">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C626" t="s">
         <v>652</v>
@@ -21189,7 +21189,7 @@
         <v>57</v>
       </c>
       <c r="B627">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C627" t="s">
         <v>653</v>
@@ -21215,7 +21215,7 @@
         <v>57</v>
       </c>
       <c r="B628">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C628" t="s">
         <v>654</v>
@@ -21241,7 +21241,7 @@
         <v>57</v>
       </c>
       <c r="B629">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C629" t="s">
         <v>655</v>
@@ -21267,7 +21267,7 @@
         <v>57</v>
       </c>
       <c r="B630">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C630" t="s">
         <v>656</v>
@@ -21293,7 +21293,7 @@
         <v>57</v>
       </c>
       <c r="B631">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C631" t="s">
         <v>657</v>
@@ -21319,7 +21319,7 @@
         <v>57</v>
       </c>
       <c r="B632">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C632" t="s">
         <v>658</v>
@@ -21345,7 +21345,7 @@
         <v>57</v>
       </c>
       <c r="B633">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C633" t="s">
         <v>659</v>
@@ -21371,7 +21371,7 @@
         <v>57</v>
       </c>
       <c r="B634">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C634" t="s">
         <v>660</v>
@@ -21397,7 +21397,7 @@
         <v>57</v>
       </c>
       <c r="B635">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C635" t="s">
         <v>661</v>
@@ -21423,7 +21423,7 @@
         <v>57</v>
       </c>
       <c r="B636">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C636" t="s">
         <v>662</v>
@@ -21449,7 +21449,7 @@
         <v>57</v>
       </c>
       <c r="B637">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C637" t="s">
         <v>663</v>
@@ -21475,7 +21475,7 @@
         <v>56</v>
       </c>
       <c r="B638">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C638" t="s">
         <v>664</v>
@@ -21501,7 +21501,7 @@
         <v>56</v>
       </c>
       <c r="B639">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C639" t="s">
         <v>665</v>
@@ -21527,7 +21527,7 @@
         <v>56</v>
       </c>
       <c r="B640">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C640" t="s">
         <v>666</v>
@@ -21553,7 +21553,7 @@
         <v>56</v>
       </c>
       <c r="B641">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C641" t="s">
         <v>667</v>
@@ -21579,7 +21579,7 @@
         <v>56</v>
       </c>
       <c r="B642">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C642" t="s">
         <v>668</v>
@@ -21605,7 +21605,7 @@
         <v>56</v>
       </c>
       <c r="B643">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C643" t="s">
         <v>669</v>
@@ -21631,7 +21631,7 @@
         <v>56</v>
       </c>
       <c r="B644">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C644" t="s">
         <v>670</v>
@@ -21657,7 +21657,7 @@
         <v>56</v>
       </c>
       <c r="B645">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C645" t="s">
         <v>671</v>
@@ -21683,7 +21683,7 @@
         <v>56</v>
       </c>
       <c r="B646">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C646" t="s">
         <v>672</v>
@@ -21709,7 +21709,7 @@
         <v>56</v>
       </c>
       <c r="B647">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C647" t="s">
         <v>673</v>
@@ -21735,7 +21735,7 @@
         <v>56</v>
       </c>
       <c r="B648">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C648" t="s">
         <v>674</v>
@@ -21761,7 +21761,7 @@
         <v>56</v>
       </c>
       <c r="B649">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C649" t="s">
         <v>675</v>
@@ -21787,7 +21787,7 @@
         <v>56</v>
       </c>
       <c r="B650">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C650" t="s">
         <v>676</v>
@@ -21813,7 +21813,7 @@
         <v>56</v>
       </c>
       <c r="B651">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C651" t="s">
         <v>677</v>
@@ -21839,7 +21839,7 @@
         <v>56</v>
       </c>
       <c r="B652">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C652" t="s">
         <v>678</v>
@@ -21865,7 +21865,7 @@
         <v>56</v>
       </c>
       <c r="B653">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C653" t="s">
         <v>679</v>
@@ -21891,7 +21891,7 @@
         <v>56</v>
       </c>
       <c r="B654">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C654" t="s">
         <v>680</v>
@@ -21917,7 +21917,7 @@
         <v>56</v>
       </c>
       <c r="B655">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C655" t="s">
         <v>681</v>
@@ -21943,7 +21943,7 @@
         <v>56</v>
       </c>
       <c r="B656">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C656" t="s">
         <v>682</v>
@@ -21969,7 +21969,7 @@
         <v>56</v>
       </c>
       <c r="B657">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C657" t="s">
         <v>683</v>
@@ -21995,7 +21995,7 @@
         <v>56</v>
       </c>
       <c r="B658">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C658" t="s">
         <v>684</v>
@@ -22021,7 +22021,7 @@
         <v>56</v>
       </c>
       <c r="B659">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C659" t="s">
         <v>685</v>
@@ -22047,7 +22047,7 @@
         <v>56</v>
       </c>
       <c r="B660">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C660" t="s">
         <v>686</v>
@@ -22073,7 +22073,7 @@
         <v>56</v>
       </c>
       <c r="B661">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C661" t="s">
         <v>687</v>
@@ -22099,7 +22099,7 @@
         <v>56</v>
       </c>
       <c r="B662">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C662" t="s">
         <v>688</v>
@@ -22125,7 +22125,7 @@
         <v>56</v>
       </c>
       <c r="B663">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C663" t="s">
         <v>689</v>
@@ -22151,7 +22151,7 @@
         <v>56</v>
       </c>
       <c r="B664">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C664" t="s">
         <v>690</v>
@@ -22177,7 +22177,7 @@
         <v>56</v>
       </c>
       <c r="B665">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C665" t="s">
         <v>691</v>
@@ -22203,7 +22203,7 @@
         <v>56</v>
       </c>
       <c r="B666">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C666" t="s">
         <v>692</v>
@@ -22229,7 +22229,7 @@
         <v>56</v>
       </c>
       <c r="B667">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C667" t="s">
         <v>693</v>
@@ -22255,7 +22255,7 @@
         <v>56</v>
       </c>
       <c r="B668">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C668" t="s">
         <v>694</v>
@@ -22281,7 +22281,7 @@
         <v>56</v>
       </c>
       <c r="B669">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C669" t="s">
         <v>695</v>
@@ -22307,7 +22307,7 @@
         <v>56</v>
       </c>
       <c r="B670">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C670" t="s">
         <v>696</v>
@@ -22333,7 +22333,7 @@
         <v>56</v>
       </c>
       <c r="B671">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C671" t="s">
         <v>697</v>
@@ -22359,7 +22359,7 @@
         <v>56</v>
       </c>
       <c r="B672">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C672" t="s">
         <v>698</v>
@@ -22385,7 +22385,7 @@
         <v>56</v>
       </c>
       <c r="B673">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C673" t="s">
         <v>699</v>
@@ -22411,7 +22411,7 @@
         <v>56</v>
       </c>
       <c r="B674">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C674" t="s">
         <v>700</v>
@@ -22437,7 +22437,7 @@
         <v>56</v>
       </c>
       <c r="B675">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C675" t="s">
         <v>701</v>
@@ -22463,7 +22463,7 @@
         <v>56</v>
       </c>
       <c r="B676">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C676" t="s">
         <v>702</v>
@@ -22489,7 +22489,7 @@
         <v>56</v>
       </c>
       <c r="B677">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C677" t="s">
         <v>703</v>
@@ -22515,7 +22515,7 @@
         <v>56</v>
       </c>
       <c r="B678">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C678" t="s">
         <v>704</v>
@@ -22541,7 +22541,7 @@
         <v>56</v>
       </c>
       <c r="B679">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C679" t="s">
         <v>705</v>
@@ -22567,7 +22567,7 @@
         <v>56</v>
       </c>
       <c r="B680">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C680" t="s">
         <v>706</v>
@@ -22593,7 +22593,7 @@
         <v>56</v>
       </c>
       <c r="B681">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C681" t="s">
         <v>707</v>
@@ -22619,7 +22619,7 @@
         <v>56</v>
       </c>
       <c r="B682">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C682" t="s">
         <v>708</v>
@@ -22645,7 +22645,7 @@
         <v>56</v>
       </c>
       <c r="B683">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C683" t="s">
         <v>709</v>
@@ -22671,7 +22671,7 @@
         <v>56</v>
       </c>
       <c r="B684">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C684" t="s">
         <v>710</v>
@@ -22697,7 +22697,7 @@
         <v>56</v>
       </c>
       <c r="B685">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C685" t="s">
         <v>711</v>
@@ -22723,7 +22723,7 @@
         <v>56</v>
       </c>
       <c r="B686">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C686" t="s">
         <v>712</v>
@@ -22749,7 +22749,7 @@
         <v>56</v>
       </c>
       <c r="B687">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C687" t="s">
         <v>713</v>
@@ -22775,7 +22775,7 @@
         <v>56</v>
       </c>
       <c r="B688">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C688" t="s">
         <v>714</v>
@@ -22801,7 +22801,7 @@
         <v>56</v>
       </c>
       <c r="B689">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C689" t="s">
         <v>715</v>
@@ -22827,7 +22827,7 @@
         <v>56</v>
       </c>
       <c r="B690">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C690" t="s">
         <v>715</v>
@@ -22853,7 +22853,7 @@
         <v>56</v>
       </c>
       <c r="B691">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C691" t="s">
         <v>716</v>
@@ -22879,7 +22879,7 @@
         <v>56</v>
       </c>
       <c r="B692">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C692" t="s">
         <v>717</v>
@@ -22905,7 +22905,7 @@
         <v>56</v>
       </c>
       <c r="B693">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C693" t="s">
         <v>718</v>
@@ -22931,7 +22931,7 @@
         <v>56</v>
       </c>
       <c r="B694">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C694" t="s">
         <v>719</v>
@@ -22957,7 +22957,7 @@
         <v>56</v>
       </c>
       <c r="B695">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C695" t="s">
         <v>720</v>
@@ -22983,7 +22983,7 @@
         <v>56</v>
       </c>
       <c r="B696">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C696" t="s">
         <v>721</v>
@@ -23009,7 +23009,7 @@
         <v>56</v>
       </c>
       <c r="B697">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C697" t="s">
         <v>722</v>
@@ -23035,7 +23035,7 @@
         <v>56</v>
       </c>
       <c r="B698">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C698" t="s">
         <v>723</v>
@@ -23061,7 +23061,7 @@
         <v>56</v>
       </c>
       <c r="B699">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C699" t="s">
         <v>724</v>
@@ -23087,7 +23087,7 @@
         <v>56</v>
       </c>
       <c r="B700">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C700" t="s">
         <v>725</v>
@@ -23113,7 +23113,7 @@
         <v>56</v>
       </c>
       <c r="B701">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C701" t="s">
         <v>726</v>
@@ -23139,7 +23139,7 @@
         <v>56</v>
       </c>
       <c r="B702">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C702" t="s">
         <v>727</v>
@@ -23165,7 +23165,7 @@
         <v>56</v>
       </c>
       <c r="B703">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C703" t="s">
         <v>728</v>
@@ -23191,7 +23191,7 @@
         <v>56</v>
       </c>
       <c r="B704">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C704" t="s">
         <v>729</v>
@@ -23217,7 +23217,7 @@
         <v>56</v>
       </c>
       <c r="B705">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C705" t="s">
         <v>730</v>
@@ -23243,7 +23243,7 @@
         <v>56</v>
       </c>
       <c r="B706">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C706" t="s">
         <v>731</v>
@@ -23269,7 +23269,7 @@
         <v>56</v>
       </c>
       <c r="B707">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C707" t="s">
         <v>732</v>
@@ -23295,7 +23295,7 @@
         <v>56</v>
       </c>
       <c r="B708">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C708" t="s">
         <v>733</v>
@@ -23321,7 +23321,7 @@
         <v>56</v>
       </c>
       <c r="B709">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C709" t="s">
         <v>734</v>
@@ -23347,7 +23347,7 @@
         <v>56</v>
       </c>
       <c r="B710">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C710" t="s">
         <v>735</v>
@@ -23373,7 +23373,7 @@
         <v>56</v>
       </c>
       <c r="B711">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C711" t="s">
         <v>736</v>
@@ -23399,7 +23399,7 @@
         <v>56</v>
       </c>
       <c r="B712">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C712" t="s">
         <v>737</v>
@@ -23425,7 +23425,7 @@
         <v>56</v>
       </c>
       <c r="B713">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C713" t="s">
         <v>738</v>
@@ -23451,7 +23451,7 @@
         <v>56</v>
       </c>
       <c r="B714">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C714" t="s">
         <v>739</v>
@@ -23477,7 +23477,7 @@
         <v>56</v>
       </c>
       <c r="B715">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C715" t="s">
         <v>740</v>
@@ -23503,7 +23503,7 @@
         <v>55</v>
       </c>
       <c r="B716">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C716" t="s">
         <v>741</v>
@@ -23535,7 +23535,7 @@
         <v>55</v>
       </c>
       <c r="B717">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C717" t="s">
         <v>743</v>
@@ -23561,7 +23561,7 @@
         <v>55</v>
       </c>
       <c r="B718">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C718" t="s">
         <v>742</v>
@@ -23587,7 +23587,7 @@
         <v>55</v>
       </c>
       <c r="B719">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C719" t="s">
         <v>744</v>
@@ -23613,7 +23613,7 @@
         <v>55</v>
       </c>
       <c r="B720">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C720" t="s">
         <v>745</v>
@@ -23639,7 +23639,7 @@
         <v>55</v>
       </c>
       <c r="B721">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C721" t="s">
         <v>746</v>
@@ -23665,7 +23665,7 @@
         <v>55</v>
       </c>
       <c r="B722">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C722" t="s">
         <v>747</v>
@@ -23691,7 +23691,7 @@
         <v>55</v>
       </c>
       <c r="B723">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C723" t="s">
         <v>748</v>
@@ -23717,7 +23717,7 @@
         <v>55</v>
       </c>
       <c r="B724">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C724" t="s">
         <v>749</v>
@@ -23743,7 +23743,7 @@
         <v>55</v>
       </c>
       <c r="B725">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C725" t="s">
         <v>750</v>
@@ -23769,7 +23769,7 @@
         <v>55</v>
       </c>
       <c r="B726">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C726" t="s">
         <v>751</v>
@@ -23795,7 +23795,7 @@
         <v>55</v>
       </c>
       <c r="B727">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C727" t="s">
         <v>752</v>
@@ -23821,7 +23821,7 @@
         <v>55</v>
       </c>
       <c r="B728">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C728" t="s">
         <v>753</v>
@@ -23847,7 +23847,7 @@
         <v>55</v>
       </c>
       <c r="B729">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C729" t="s">
         <v>754</v>
@@ -23873,7 +23873,7 @@
         <v>55</v>
       </c>
       <c r="B730">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C730" t="s">
         <v>755</v>
@@ -23899,7 +23899,7 @@
         <v>55</v>
       </c>
       <c r="B731">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C731" t="s">
         <v>756</v>
@@ -23925,7 +23925,7 @@
         <v>55</v>
       </c>
       <c r="B732">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C732" t="s">
         <v>757</v>
@@ -23951,7 +23951,7 @@
         <v>55</v>
       </c>
       <c r="B733">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C733" t="s">
         <v>758</v>
@@ -23977,7 +23977,7 @@
         <v>55</v>
       </c>
       <c r="B734">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C734" t="s">
         <v>759</v>
@@ -24003,7 +24003,7 @@
         <v>55</v>
       </c>
       <c r="B735">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C735" t="s">
         <v>760</v>
@@ -24029,7 +24029,7 @@
         <v>55</v>
       </c>
       <c r="B736">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C736" t="s">
         <v>761</v>
@@ -24055,7 +24055,7 @@
         <v>55</v>
       </c>
       <c r="B737">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C737" t="s">
         <v>762</v>
@@ -24081,7 +24081,7 @@
         <v>55</v>
       </c>
       <c r="B738">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C738" t="s">
         <v>763</v>
@@ -24107,7 +24107,7 @@
         <v>55</v>
       </c>
       <c r="B739">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C739" t="s">
         <v>764</v>
@@ -24133,7 +24133,7 @@
         <v>55</v>
       </c>
       <c r="B740">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C740" t="s">
         <v>765</v>
@@ -24159,7 +24159,7 @@
         <v>55</v>
       </c>
       <c r="B741">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C741" t="s">
         <v>766</v>
@@ -24185,7 +24185,7 @@
         <v>55</v>
       </c>
       <c r="B742">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C742" t="s">
         <v>767</v>
@@ -24211,7 +24211,7 @@
         <v>55</v>
       </c>
       <c r="B743">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C743" t="s">
         <v>768</v>
@@ -24237,7 +24237,7 @@
         <v>55</v>
       </c>
       <c r="B744">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C744" t="s">
         <v>769</v>
@@ -24263,7 +24263,7 @@
         <v>55</v>
       </c>
       <c r="B745">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C745" t="s">
         <v>770</v>
@@ -24289,7 +24289,7 @@
         <v>55</v>
       </c>
       <c r="B746">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C746" t="s">
         <v>771</v>
@@ -24315,7 +24315,7 @@
         <v>55</v>
       </c>
       <c r="B747">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C747" t="s">
         <v>772</v>
@@ -24341,7 +24341,7 @@
         <v>55</v>
       </c>
       <c r="B748">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C748" t="s">
         <v>773</v>
@@ -24367,7 +24367,7 @@
         <v>55</v>
       </c>
       <c r="B749">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C749" t="s">
         <v>774</v>
@@ -24393,7 +24393,7 @@
         <v>55</v>
       </c>
       <c r="B750">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C750" t="s">
         <v>775</v>
@@ -24419,7 +24419,7 @@
         <v>55</v>
       </c>
       <c r="B751">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C751" t="s">
         <v>776</v>
@@ -24445,7 +24445,7 @@
         <v>55</v>
       </c>
       <c r="B752">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C752" t="s">
         <v>777</v>
@@ -24471,7 +24471,7 @@
         <v>55</v>
       </c>
       <c r="B753">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C753" t="s">
         <v>778</v>
@@ -24497,7 +24497,7 @@
         <v>55</v>
       </c>
       <c r="B754">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C754" t="s">
         <v>779</v>
@@ -24523,7 +24523,7 @@
         <v>55</v>
       </c>
       <c r="B755">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C755" t="s">
         <v>781</v>
@@ -24549,7 +24549,7 @@
         <v>55</v>
       </c>
       <c r="B756">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C756" t="s">
         <v>780</v>
@@ -24575,7 +24575,7 @@
         <v>55</v>
       </c>
       <c r="B757">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C757" t="s">
         <v>782</v>
@@ -24601,7 +24601,7 @@
         <v>55</v>
       </c>
       <c r="B758">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C758" t="s">
         <v>783</v>
@@ -24627,7 +24627,7 @@
         <v>55</v>
       </c>
       <c r="B759">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C759" t="s">
         <v>784</v>
@@ -24653,7 +24653,7 @@
         <v>55</v>
       </c>
       <c r="B760">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C760" t="s">
         <v>785</v>
@@ -24679,7 +24679,7 @@
         <v>55</v>
       </c>
       <c r="B761">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C761" t="s">
         <v>786</v>
@@ -24705,7 +24705,7 @@
         <v>55</v>
       </c>
       <c r="B762">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C762" t="s">
         <v>787</v>
@@ -24731,7 +24731,7 @@
         <v>55</v>
       </c>
       <c r="B763">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C763" t="s">
         <v>788</v>
@@ -24757,7 +24757,7 @@
         <v>55</v>
       </c>
       <c r="B764">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C764" t="s">
         <v>789</v>
@@ -24783,7 +24783,7 @@
         <v>55</v>
       </c>
       <c r="B765">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C765" t="s">
         <v>790</v>
@@ -24809,7 +24809,7 @@
         <v>55</v>
       </c>
       <c r="B766">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C766" t="s">
         <v>791</v>
@@ -24835,7 +24835,7 @@
         <v>55</v>
       </c>
       <c r="B767">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C767" t="s">
         <v>792</v>
@@ -24861,7 +24861,7 @@
         <v>55</v>
       </c>
       <c r="B768">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C768" t="s">
         <v>793</v>
@@ -24887,7 +24887,7 @@
         <v>55</v>
       </c>
       <c r="B769">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C769" t="s">
         <v>794</v>
@@ -24913,7 +24913,7 @@
         <v>55</v>
       </c>
       <c r="B770">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C770" t="s">
         <v>795</v>
@@ -24939,7 +24939,7 @@
         <v>55</v>
       </c>
       <c r="B771">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C771" t="s">
         <v>796</v>
@@ -24965,7 +24965,7 @@
         <v>55</v>
       </c>
       <c r="B772">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C772" t="s">
         <v>797</v>
@@ -24991,7 +24991,7 @@
         <v>55</v>
       </c>
       <c r="B773">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C773" t="s">
         <v>134</v>
@@ -25017,7 +25017,7 @@
         <v>55</v>
       </c>
       <c r="B774">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C774" t="s">
         <v>798</v>
@@ -25043,7 +25043,7 @@
         <v>55</v>
       </c>
       <c r="B775">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C775" t="s">
         <v>799</v>
@@ -25069,7 +25069,7 @@
         <v>55</v>
       </c>
       <c r="B776">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C776" t="s">
         <v>800</v>
@@ -25095,7 +25095,7 @@
         <v>55</v>
       </c>
       <c r="B777">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C777" t="s">
         <v>801</v>
@@ -25121,7 +25121,7 @@
         <v>55</v>
       </c>
       <c r="B778">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C778" t="s">
         <v>802</v>
@@ -25147,7 +25147,7 @@
         <v>55</v>
       </c>
       <c r="B779">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C779" t="s">
         <v>803</v>
@@ -25173,7 +25173,7 @@
         <v>55</v>
       </c>
       <c r="B780">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C780" t="s">
         <v>804</v>
@@ -25199,7 +25199,7 @@
         <v>55</v>
       </c>
       <c r="B781">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C781" t="s">
         <v>805</v>
@@ -25225,7 +25225,7 @@
         <v>55</v>
       </c>
       <c r="B782">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C782" t="s">
         <v>806</v>
@@ -25251,7 +25251,7 @@
         <v>55</v>
       </c>
       <c r="B783">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C783" t="s">
         <v>807</v>
@@ -25277,7 +25277,7 @@
         <v>55</v>
       </c>
       <c r="B784">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C784" t="s">
         <v>808</v>
@@ -25303,7 +25303,7 @@
         <v>55</v>
       </c>
       <c r="B785">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C785" t="s">
         <v>809</v>
@@ -25329,7 +25329,7 @@
         <v>55</v>
       </c>
       <c r="B786">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C786" t="s">
         <v>810</v>
@@ -25355,7 +25355,7 @@
         <v>55</v>
       </c>
       <c r="B787">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C787" t="s">
         <v>811</v>
@@ -25381,7 +25381,7 @@
         <v>55</v>
       </c>
       <c r="B788">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C788" t="s">
         <v>812</v>
@@ -25407,7 +25407,7 @@
         <v>55</v>
       </c>
       <c r="B789">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C789" t="s">
         <v>813</v>
@@ -25433,7 +25433,7 @@
         <v>55</v>
       </c>
       <c r="B790">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C790" t="s">
         <v>814</v>
@@ -25459,7 +25459,7 @@
         <v>55</v>
       </c>
       <c r="B791">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C791" t="s">
         <v>815</v>
@@ -25485,7 +25485,7 @@
         <v>55</v>
       </c>
       <c r="B792">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C792" t="s">
         <v>816</v>
@@ -25511,7 +25511,7 @@
         <v>55</v>
       </c>
       <c r="B793">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C793" t="s">
         <v>817</v>
@@ -25537,7 +25537,7 @@
         <v>55</v>
       </c>
       <c r="B794">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C794" t="s">
         <v>818</v>
@@ -25563,7 +25563,7 @@
         <v>54</v>
       </c>
       <c r="B795">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C795" t="s">
         <v>819</v>
@@ -25589,7 +25589,7 @@
         <v>54</v>
       </c>
       <c r="B796">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C796" t="s">
         <v>820</v>
@@ -25615,7 +25615,7 @@
         <v>54</v>
       </c>
       <c r="B797">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C797" t="s">
         <v>821</v>
@@ -25641,7 +25641,7 @@
         <v>54</v>
       </c>
       <c r="B798">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C798" t="s">
         <v>822</v>
@@ -25667,7 +25667,7 @@
         <v>54</v>
       </c>
       <c r="B799">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C799" t="s">
         <v>823</v>
@@ -25693,7 +25693,7 @@
         <v>54</v>
       </c>
       <c r="B800">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C800" t="s">
         <v>824</v>
@@ -25719,7 +25719,7 @@
         <v>54</v>
       </c>
       <c r="B801">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C801" t="s">
         <v>825</v>
@@ -25745,7 +25745,7 @@
         <v>54</v>
       </c>
       <c r="B802">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C802" t="s">
         <v>826</v>
@@ -25771,7 +25771,7 @@
         <v>54</v>
       </c>
       <c r="B803">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C803" t="s">
         <v>827</v>
@@ -25797,7 +25797,7 @@
         <v>54</v>
       </c>
       <c r="B804">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C804" t="s">
         <v>828</v>
@@ -25823,7 +25823,7 @@
         <v>54</v>
       </c>
       <c r="B805">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C805" t="s">
         <v>829</v>
@@ -25849,7 +25849,7 @@
         <v>54</v>
       </c>
       <c r="B806">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C806" t="s">
         <v>830</v>
@@ -25875,7 +25875,7 @@
         <v>54</v>
       </c>
       <c r="B807">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C807" t="s">
         <v>831</v>
@@ -25901,7 +25901,7 @@
         <v>54</v>
       </c>
       <c r="B808">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C808" t="s">
         <v>832</v>
@@ -25927,7 +25927,7 @@
         <v>54</v>
       </c>
       <c r="B809">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C809" t="s">
         <v>833</v>
@@ -25953,7 +25953,7 @@
         <v>54</v>
       </c>
       <c r="B810">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C810" t="s">
         <v>834</v>
@@ -25979,7 +25979,7 @@
         <v>54</v>
       </c>
       <c r="B811">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C811" t="s">
         <v>835</v>
@@ -26005,7 +26005,7 @@
         <v>54</v>
       </c>
       <c r="B812">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C812" t="s">
         <v>836</v>
@@ -26031,7 +26031,7 @@
         <v>54</v>
       </c>
       <c r="B813">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C813" t="s">
         <v>837</v>
@@ -26057,7 +26057,7 @@
         <v>54</v>
       </c>
       <c r="B814">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C814" t="s">
         <v>838</v>
@@ -26083,7 +26083,7 @@
         <v>54</v>
       </c>
       <c r="B815">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C815" t="s">
         <v>839</v>
@@ -26109,7 +26109,7 @@
         <v>54</v>
       </c>
       <c r="B816">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C816" t="s">
         <v>840</v>
@@ -26135,7 +26135,7 @@
         <v>54</v>
       </c>
       <c r="B817">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C817" t="s">
         <v>841</v>
@@ -26161,7 +26161,7 @@
         <v>54</v>
       </c>
       <c r="B818">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C818" t="s">
         <v>842</v>
@@ -26187,7 +26187,7 @@
         <v>54</v>
       </c>
       <c r="B819">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C819" t="s">
         <v>843</v>
@@ -26213,7 +26213,7 @@
         <v>54</v>
       </c>
       <c r="B820">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C820" t="s">
         <v>844</v>
@@ -26239,7 +26239,7 @@
         <v>54</v>
       </c>
       <c r="B821">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C821" t="s">
         <v>845</v>
@@ -26265,7 +26265,7 @@
         <v>54</v>
       </c>
       <c r="B822">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C822" t="s">
         <v>846</v>
@@ -26291,7 +26291,7 @@
         <v>54</v>
       </c>
       <c r="B823">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C823" t="s">
         <v>847</v>
@@ -26317,7 +26317,7 @@
         <v>54</v>
       </c>
       <c r="B824">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C824" t="s">
         <v>848</v>
@@ -26343,7 +26343,7 @@
         <v>54</v>
       </c>
       <c r="B825">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C825" t="s">
         <v>849</v>
@@ -26369,7 +26369,7 @@
         <v>54</v>
       </c>
       <c r="B826">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C826" t="s">
         <v>850</v>
@@ -26395,7 +26395,7 @@
         <v>54</v>
       </c>
       <c r="B827">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C827" t="s">
         <v>851</v>
@@ -26421,7 +26421,7 @@
         <v>54</v>
       </c>
       <c r="B828">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C828" t="s">
         <v>852</v>
@@ -26447,7 +26447,7 @@
         <v>54</v>
       </c>
       <c r="B829">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C829" t="s">
         <v>853</v>
@@ -26473,7 +26473,7 @@
         <v>54</v>
       </c>
       <c r="B830">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C830" t="s">
         <v>854</v>
@@ -26499,7 +26499,7 @@
         <v>54</v>
       </c>
       <c r="B831">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C831" t="s">
         <v>855</v>
@@ -26525,7 +26525,7 @@
         <v>54</v>
       </c>
       <c r="B832">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C832" t="s">
         <v>856</v>
@@ -26551,7 +26551,7 @@
         <v>54</v>
       </c>
       <c r="B833">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C833" t="s">
         <v>857</v>
@@ -26577,7 +26577,7 @@
         <v>54</v>
       </c>
       <c r="B834">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C834" t="s">
         <v>858</v>
@@ -26603,7 +26603,7 @@
         <v>54</v>
       </c>
       <c r="B835">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C835" t="s">
         <v>859</v>
@@ -26629,7 +26629,7 @@
         <v>54</v>
       </c>
       <c r="B836">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C836" t="s">
         <v>860</v>
@@ -26655,7 +26655,7 @@
         <v>54</v>
       </c>
       <c r="B837">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C837" t="s">
         <v>861</v>
@@ -26681,7 +26681,7 @@
         <v>54</v>
       </c>
       <c r="B838">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C838" t="s">
         <v>862</v>
@@ -26707,7 +26707,7 @@
         <v>54</v>
       </c>
       <c r="B839">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C839" t="s">
         <v>863</v>
@@ -26733,7 +26733,7 @@
         <v>54</v>
       </c>
       <c r="B840">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C840" t="s">
         <v>864</v>
@@ -26759,7 +26759,7 @@
         <v>54</v>
       </c>
       <c r="B841">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C841" t="s">
         <v>865</v>
@@ -26785,7 +26785,7 @@
         <v>54</v>
       </c>
       <c r="B842">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C842" t="s">
         <v>866</v>
@@ -26811,7 +26811,7 @@
         <v>54</v>
       </c>
       <c r="B843">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C843" t="s">
         <v>867</v>
@@ -26837,7 +26837,7 @@
         <v>54</v>
       </c>
       <c r="B844">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C844" t="s">
         <v>868</v>
@@ -26863,7 +26863,7 @@
         <v>54</v>
       </c>
       <c r="B845">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C845" t="s">
         <v>869</v>
@@ -26889,7 +26889,7 @@
         <v>54</v>
       </c>
       <c r="B846">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C846" t="s">
         <v>870</v>
@@ -26915,7 +26915,7 @@
         <v>54</v>
       </c>
       <c r="B847">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C847" t="s">
         <v>871</v>
@@ -26941,7 +26941,7 @@
         <v>54</v>
       </c>
       <c r="B848">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C848" t="s">
         <v>872</v>
@@ -26967,7 +26967,7 @@
         <v>54</v>
       </c>
       <c r="B849">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C849" t="s">
         <v>873</v>
@@ -26993,7 +26993,7 @@
         <v>54</v>
       </c>
       <c r="B850">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C850" t="s">
         <v>874</v>
@@ -27019,7 +27019,7 @@
         <v>54</v>
       </c>
       <c r="B851">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C851" t="s">
         <v>875</v>
@@ -27045,7 +27045,7 @@
         <v>54</v>
       </c>
       <c r="B852">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C852" t="s">
         <v>876</v>
@@ -27071,7 +27071,7 @@
         <v>54</v>
       </c>
       <c r="B853">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C853" t="s">
         <v>877</v>
@@ -27097,7 +27097,7 @@
         <v>54</v>
       </c>
       <c r="B854">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C854" t="s">
         <v>878</v>
@@ -27123,7 +27123,7 @@
         <v>54</v>
       </c>
       <c r="B855">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C855" t="s">
         <v>879</v>
@@ -27149,7 +27149,7 @@
         <v>54</v>
       </c>
       <c r="B856">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C856" t="s">
         <v>880</v>
@@ -27175,7 +27175,7 @@
         <v>54</v>
       </c>
       <c r="B857">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C857" t="s">
         <v>881</v>
@@ -27201,7 +27201,7 @@
         <v>54</v>
       </c>
       <c r="B858">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C858" t="s">
         <v>882</v>
@@ -27227,7 +27227,7 @@
         <v>54</v>
       </c>
       <c r="B859">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C859" t="s">
         <v>883</v>
@@ -27253,7 +27253,7 @@
         <v>54</v>
       </c>
       <c r="B860">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C860" t="s">
         <v>884</v>
@@ -27279,7 +27279,7 @@
         <v>54</v>
       </c>
       <c r="B861">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C861" t="s">
         <v>885</v>
@@ -27305,7 +27305,7 @@
         <v>54</v>
       </c>
       <c r="B862">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C862" t="s">
         <v>886</v>
@@ -27331,7 +27331,7 @@
         <v>54</v>
       </c>
       <c r="B863">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C863" t="s">
         <v>887</v>
@@ -27357,7 +27357,7 @@
         <v>54</v>
       </c>
       <c r="B864">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C864" t="s">
         <v>888</v>
@@ -27383,7 +27383,7 @@
         <v>54</v>
       </c>
       <c r="B865">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C865" t="s">
         <v>889</v>
@@ -27409,7 +27409,7 @@
         <v>54</v>
       </c>
       <c r="B866">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C866" t="s">
         <v>890</v>
@@ -27435,7 +27435,7 @@
         <v>54</v>
       </c>
       <c r="B867">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C867" t="s">
         <v>891</v>
@@ -27461,7 +27461,7 @@
         <v>54</v>
       </c>
       <c r="B868">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C868" t="s">
         <v>892</v>
@@ -27487,7 +27487,7 @@
         <v>54</v>
       </c>
       <c r="B869">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C869" t="s">
         <v>893</v>
@@ -27513,7 +27513,7 @@
         <v>54</v>
       </c>
       <c r="B870">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C870" t="s">
         <v>894</v>
@@ -27539,7 +27539,7 @@
         <v>54</v>
       </c>
       <c r="B871">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C871" t="s">
         <v>895</v>
@@ -27565,7 +27565,7 @@
         <v>54</v>
       </c>
       <c r="B872">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C872" t="s">
         <v>896</v>
@@ -27591,7 +27591,7 @@
         <v>54</v>
       </c>
       <c r="B873">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C873" t="s">
         <v>897</v>
@@ -27617,7 +27617,7 @@
         <v>54</v>
       </c>
       <c r="B874">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C874" t="s">
         <v>898</v>
@@ -27643,7 +27643,7 @@
         <v>53</v>
       </c>
       <c r="B875">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C875" t="s">
         <v>899</v>
@@ -27669,7 +27669,7 @@
         <v>53</v>
       </c>
       <c r="B876">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C876" t="s">
         <v>900</v>
@@ -27695,7 +27695,7 @@
         <v>53</v>
       </c>
       <c r="B877">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C877" t="s">
         <v>901</v>
@@ -27721,7 +27721,7 @@
         <v>53</v>
       </c>
       <c r="B878">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C878" t="s">
         <v>902</v>
@@ -27747,7 +27747,7 @@
         <v>53</v>
       </c>
       <c r="B879">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C879" t="s">
         <v>903</v>
@@ -27773,7 +27773,7 @@
         <v>53</v>
       </c>
       <c r="B880">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C880" t="s">
         <v>904</v>
@@ -27799,7 +27799,7 @@
         <v>53</v>
       </c>
       <c r="B881">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C881" t="s">
         <v>905</v>
@@ -27825,7 +27825,7 @@
         <v>53</v>
       </c>
       <c r="B882">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C882" t="s">
         <v>906</v>
@@ -27851,7 +27851,7 @@
         <v>53</v>
       </c>
       <c r="B883">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C883" t="s">
         <v>907</v>
@@ -27877,7 +27877,7 @@
         <v>53</v>
       </c>
       <c r="B884">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C884" t="s">
         <v>908</v>
@@ -27903,7 +27903,7 @@
         <v>53</v>
       </c>
       <c r="B885">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C885" t="s">
         <v>909</v>
@@ -27929,7 +27929,7 @@
         <v>53</v>
       </c>
       <c r="B886">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C886" t="s">
         <v>910</v>
@@ -27955,7 +27955,7 @@
         <v>53</v>
       </c>
       <c r="B887">
-        <v>1804</v>
+        <v>1904</v>
       </c>
       <c r="C887" t="s">
         <v>911</v>

</xml_diff>

<commit_message>
confirmacions any 1879 completes
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Confirmacions/Excel/Index_Llibres_Confirmacions_Linyola.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Confirmacions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E74A3F-3EBE-4EAC-B48B-398A0740FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2F32D-A293-4CAB-ADB7-11EF87172BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FEEAE0F-87B7-4CFD-9217-CD5D622A9875}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8438" uniqueCount="1710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8860" uniqueCount="1781">
   <si>
     <t>Cognons</t>
   </si>
@@ -5170,6 +5170,219 @@
   </si>
   <si>
     <t>Fabregat Miquel Dolors</t>
+  </si>
+  <si>
+    <t>Solé Ginestà Sebastià</t>
+  </si>
+  <si>
+    <t>Ginestà Gilabert Marceli</t>
+  </si>
+  <si>
+    <t>Sisteró Palomés Ramon</t>
+  </si>
+  <si>
+    <t>Batlle Brescó Josep</t>
+  </si>
+  <si>
+    <t>Torrent Lamarca Sebastià</t>
+  </si>
+  <si>
+    <t>Roca Camrubí Jaume</t>
+  </si>
+  <si>
+    <t>Escolà Pascual Josep</t>
+  </si>
+  <si>
+    <t>Roig Mas Francisco</t>
+  </si>
+  <si>
+    <t>Martí Palou Ramon</t>
+  </si>
+  <si>
+    <t>Pujades Valls Jaume</t>
+  </si>
+  <si>
+    <t>Falcó Oró Joan</t>
+  </si>
+  <si>
+    <t>Balcells Huguet Josep Antoni</t>
+  </si>
+  <si>
+    <t>Salles Coll Francisco</t>
+  </si>
+  <si>
+    <t>Trepat Ginestà Ramon</t>
+  </si>
+  <si>
+    <t>Cistró Falcó Ramon</t>
+  </si>
+  <si>
+    <t>Coca Palou Francisco</t>
+  </si>
+  <si>
+    <t>Mosset Mas Jaume</t>
+  </si>
+  <si>
+    <t>Majoral Pallerola Josep</t>
+  </si>
+  <si>
+    <t>Pedrós Sunyé Antoni</t>
+  </si>
+  <si>
+    <t>Roca Camrubí Francisco</t>
+  </si>
+  <si>
+    <t>Duart Costafreda Joan</t>
+  </si>
+  <si>
+    <t>Duart Costafreda Josep</t>
+  </si>
+  <si>
+    <t>Vallés Roig Francisco</t>
+  </si>
+  <si>
+    <t>Escolà Formiguera Jaume</t>
+  </si>
+  <si>
+    <t>Roma Giné Ramon</t>
+  </si>
+  <si>
+    <t>Colell Pedrós Antoni</t>
+  </si>
+  <si>
+    <t>Martí Piera Silbestre</t>
+  </si>
+  <si>
+    <t>Pedra Vallés Fernando</t>
+  </si>
+  <si>
+    <t>Planes Fabregat Pau</t>
+  </si>
+  <si>
+    <t>Majoral Pallerola Manuel</t>
+  </si>
+  <si>
+    <t>Formiguera Coll Ramon</t>
+  </si>
+  <si>
+    <t>Vergé Mases Salvador</t>
+  </si>
+  <si>
+    <t>Serra Escolà Sacarias</t>
+  </si>
+  <si>
+    <t>Pedrós Morera Ignasi</t>
+  </si>
+  <si>
+    <t>Ginestà Giné Francisco</t>
+  </si>
+  <si>
+    <t>Vilamajó Duart Felip</t>
+  </si>
+  <si>
+    <t>Pedrós Prats Francisco</t>
+  </si>
+  <si>
+    <t>Pedrós Solsona Joan</t>
+  </si>
+  <si>
+    <t>Serra Escolà Antoni</t>
+  </si>
+  <si>
+    <t>Camarasa Balcells Josep</t>
+  </si>
+  <si>
+    <t>Aldomà Brescó Josep</t>
+  </si>
+  <si>
+    <t>Giné Salles Francisco</t>
+  </si>
+  <si>
+    <t>Pallerola Bondia Josep</t>
+  </si>
+  <si>
+    <t>Cercós Sunyé Pere Jaume</t>
+  </si>
+  <si>
+    <t>Formiguera Novell Joan</t>
+  </si>
+  <si>
+    <t>Fabregat Mosset Bautista</t>
+  </si>
+  <si>
+    <t>Coll Mata Domingo</t>
+  </si>
+  <si>
+    <t>Figuera Sunyé Esteve</t>
+  </si>
+  <si>
+    <t>Gispert Regtós  Jaume</t>
+  </si>
+  <si>
+    <t>Jové Carbonell Josep</t>
+  </si>
+  <si>
+    <t>Jové Carbonell Francisco</t>
+  </si>
+  <si>
+    <t>Planes Pujol Ramon</t>
+  </si>
+  <si>
+    <t>Planes Fabregat Josep</t>
+  </si>
+  <si>
+    <t>Pedrós Pujades Andreu</t>
+  </si>
+  <si>
+    <t>Martí Piera Josep</t>
+  </si>
+  <si>
+    <t>Pedrós Bresolí Antoni Ramon</t>
+  </si>
+  <si>
+    <t>Mosset Farré Antoni</t>
+  </si>
+  <si>
+    <t>Querol Casals Melinton</t>
+  </si>
+  <si>
+    <t>Miquel Querol</t>
+  </si>
+  <si>
+    <t>Maria Casals</t>
+  </si>
+  <si>
+    <t>Coll Giné Josep</t>
+  </si>
+  <si>
+    <t>Colell Pedrós Francisco</t>
+  </si>
+  <si>
+    <t>Mas Vergé Pau</t>
+  </si>
+  <si>
+    <t>Vilaplana Pallerola Antoni</t>
+  </si>
+  <si>
+    <t>Martí Trilla Miquel</t>
+  </si>
+  <si>
+    <t>Auró Codun? Joan</t>
+  </si>
+  <si>
+    <t>Duart Colell Ignasi</t>
+  </si>
+  <si>
+    <t>Cascalló Farré Esteve</t>
+  </si>
+  <si>
+    <t>Roig Mas Maties</t>
+  </si>
+  <si>
+    <t>Druet Farré Domingo</t>
+  </si>
+  <si>
+    <t>Cascalló Farré Antoni</t>
   </si>
 </sst>
 </file>
@@ -5536,10 +5749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EAC519-AAA9-4752-A1C1-63CDDDDDC53A}">
-  <dimension ref="A1:L1696"/>
+  <dimension ref="A1:L1766"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1684" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1697" sqref="A1697"/>
+    <sheetView tabSelected="1" topLeftCell="A1732" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1767" sqref="A1767"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52122,6 +52335,2042 @@
         <v>12</v>
       </c>
       <c r="K1696" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1697">
+        <v>41</v>
+      </c>
+      <c r="B1697">
+        <v>1879</v>
+      </c>
+      <c r="C1697" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F1697" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1697" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1697" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1697">
+        <v>47</v>
+      </c>
+      <c r="J1697" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1697" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1698">
+        <v>41</v>
+      </c>
+      <c r="B1698">
+        <v>1879</v>
+      </c>
+      <c r="C1698" t="s">
+        <v>1711</v>
+      </c>
+      <c r="F1698" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1698" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1698" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1698">
+        <v>47</v>
+      </c>
+      <c r="J1698" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1698" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1699">
+        <v>41</v>
+      </c>
+      <c r="B1699">
+        <v>1879</v>
+      </c>
+      <c r="C1699" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F1699" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1699" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1699" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1699">
+        <v>47</v>
+      </c>
+      <c r="J1699" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1699" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1700">
+        <v>41</v>
+      </c>
+      <c r="B1700">
+        <v>1879</v>
+      </c>
+      <c r="C1700" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1700" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1700" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1700" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1700">
+        <v>47</v>
+      </c>
+      <c r="J1700" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1700" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1701">
+        <v>41</v>
+      </c>
+      <c r="B1701">
+        <v>1879</v>
+      </c>
+      <c r="C1701" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F1701" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1701" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1701" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1701">
+        <v>47</v>
+      </c>
+      <c r="J1701" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1701" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1702">
+        <v>41</v>
+      </c>
+      <c r="B1702">
+        <v>1879</v>
+      </c>
+      <c r="C1702" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F1702" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1702" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1702" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1702">
+        <v>47</v>
+      </c>
+      <c r="J1702" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1702" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1703">
+        <v>41</v>
+      </c>
+      <c r="B1703">
+        <v>1879</v>
+      </c>
+      <c r="C1703" t="s">
+        <v>1351</v>
+      </c>
+      <c r="F1703" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1703" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1703" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1703">
+        <v>47</v>
+      </c>
+      <c r="J1703" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1703" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1704">
+        <v>41</v>
+      </c>
+      <c r="B1704">
+        <v>1879</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1704" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1704" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1704" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1704">
+        <v>47</v>
+      </c>
+      <c r="J1704" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1704" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1705">
+        <v>41</v>
+      </c>
+      <c r="B1705">
+        <v>1879</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1705" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1705" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1705" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1705">
+        <v>47</v>
+      </c>
+      <c r="J1705" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1705" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1706">
+        <v>41</v>
+      </c>
+      <c r="B1706">
+        <v>1879</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1706" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1706" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1706" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1706">
+        <v>47</v>
+      </c>
+      <c r="J1706" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1706" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1707">
+        <v>41</v>
+      </c>
+      <c r="B1707">
+        <v>1879</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1707" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1707" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1707" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1707">
+        <v>47</v>
+      </c>
+      <c r="J1707" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1707" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1708">
+        <v>41</v>
+      </c>
+      <c r="B1708">
+        <v>1879</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1708" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1708" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1708" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1708">
+        <v>47</v>
+      </c>
+      <c r="J1708" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1708" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1709">
+        <v>41</v>
+      </c>
+      <c r="B1709">
+        <v>1879</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F1709" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1709" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1709" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1709">
+        <v>47</v>
+      </c>
+      <c r="J1709" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1709" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1710">
+        <v>41</v>
+      </c>
+      <c r="B1710">
+        <v>1879</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F1710" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1710" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1710" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1710">
+        <v>47</v>
+      </c>
+      <c r="J1710" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1710" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1711">
+        <v>41</v>
+      </c>
+      <c r="B1711">
+        <v>1879</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>1723</v>
+      </c>
+      <c r="F1711" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1711" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1711" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1711">
+        <v>47</v>
+      </c>
+      <c r="J1711" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1711" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1712">
+        <v>41</v>
+      </c>
+      <c r="B1712">
+        <v>1879</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F1712" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1712" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1712" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1712">
+        <v>47</v>
+      </c>
+      <c r="J1712" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1712" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1713">
+        <v>41</v>
+      </c>
+      <c r="B1713">
+        <v>1879</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F1713" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1713" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1713" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1713">
+        <v>47</v>
+      </c>
+      <c r="J1713" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1713" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1714">
+        <v>41</v>
+      </c>
+      <c r="B1714">
+        <v>1879</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F1714" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1714" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1714" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1714">
+        <v>47</v>
+      </c>
+      <c r="J1714" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1714" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1715">
+        <v>41</v>
+      </c>
+      <c r="B1715">
+        <v>1879</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F1715" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1715" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1715" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1715">
+        <v>47</v>
+      </c>
+      <c r="J1715" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1715" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1716">
+        <v>41</v>
+      </c>
+      <c r="B1716">
+        <v>1879</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>1728</v>
+      </c>
+      <c r="F1716" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1716" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1716" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1716">
+        <v>47</v>
+      </c>
+      <c r="J1716" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1716" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1717">
+        <v>41</v>
+      </c>
+      <c r="B1717">
+        <v>1879</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>1729</v>
+      </c>
+      <c r="F1717" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1717" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1717" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1717">
+        <v>47</v>
+      </c>
+      <c r="J1717" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1717" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1718">
+        <v>41</v>
+      </c>
+      <c r="B1718">
+        <v>1879</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>1730</v>
+      </c>
+      <c r="F1718" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1718" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1718" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1718">
+        <v>47</v>
+      </c>
+      <c r="J1718" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1718" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1719">
+        <v>41</v>
+      </c>
+      <c r="B1719">
+        <v>1879</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F1719" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1719" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1719" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1719">
+        <v>47</v>
+      </c>
+      <c r="J1719" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1719" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1720">
+        <v>41</v>
+      </c>
+      <c r="B1720">
+        <v>1879</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F1720" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1720" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1720" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1720">
+        <v>47</v>
+      </c>
+      <c r="J1720" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1720" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1721">
+        <v>41</v>
+      </c>
+      <c r="B1721">
+        <v>1879</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F1721" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1721" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1721" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1721">
+        <v>47</v>
+      </c>
+      <c r="J1721" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1721" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1722">
+        <v>41</v>
+      </c>
+      <c r="B1722">
+        <v>1879</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>1734</v>
+      </c>
+      <c r="F1722" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1722" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1722" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1722">
+        <v>47</v>
+      </c>
+      <c r="J1722" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1722" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1723">
+        <v>41</v>
+      </c>
+      <c r="B1723">
+        <v>1879</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>1735</v>
+      </c>
+      <c r="F1723" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1723" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1723" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1723">
+        <v>47</v>
+      </c>
+      <c r="J1723" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1723" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1724">
+        <v>41</v>
+      </c>
+      <c r="B1724">
+        <v>1879</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F1724" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1724" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1724" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1724">
+        <v>47</v>
+      </c>
+      <c r="J1724" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1724" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1725">
+        <v>41</v>
+      </c>
+      <c r="B1725">
+        <v>1879</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F1725" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1725" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1725" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1725">
+        <v>47</v>
+      </c>
+      <c r="J1725" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1725" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1726">
+        <v>41</v>
+      </c>
+      <c r="B1726">
+        <v>1879</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F1726" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1726" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1726" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1726">
+        <v>47</v>
+      </c>
+      <c r="J1726" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1726" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1727">
+        <v>41</v>
+      </c>
+      <c r="B1727">
+        <v>1879</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F1727" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1727" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1727" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1727">
+        <v>47</v>
+      </c>
+      <c r="J1727" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1727" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1728">
+        <v>41</v>
+      </c>
+      <c r="B1728">
+        <v>1879</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F1728" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1728" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1728" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1728">
+        <v>47</v>
+      </c>
+      <c r="J1728" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1728" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1729">
+        <v>41</v>
+      </c>
+      <c r="B1729">
+        <v>1879</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F1729" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1729" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1729" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1729">
+        <v>47</v>
+      </c>
+      <c r="J1729" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1729" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1730">
+        <v>41</v>
+      </c>
+      <c r="B1730">
+        <v>1879</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F1730" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1730" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1730" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1730">
+        <v>47</v>
+      </c>
+      <c r="J1730" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1730" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1731">
+        <v>41</v>
+      </c>
+      <c r="B1731">
+        <v>1879</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F1731" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1731" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1731" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1731">
+        <v>47</v>
+      </c>
+      <c r="J1731" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1731" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1732">
+        <v>41</v>
+      </c>
+      <c r="B1732">
+        <v>1879</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F1732" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1732" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1732" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1732">
+        <v>47</v>
+      </c>
+      <c r="J1732" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1732" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1733">
+        <v>41</v>
+      </c>
+      <c r="B1733">
+        <v>1879</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>1745</v>
+      </c>
+      <c r="F1733" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1733" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1733" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1733">
+        <v>47</v>
+      </c>
+      <c r="J1733" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1733" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1734">
+        <v>41</v>
+      </c>
+      <c r="B1734">
+        <v>1879</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F1734" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1734" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1734" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1734">
+        <v>47</v>
+      </c>
+      <c r="J1734" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1734" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1735">
+        <v>41</v>
+      </c>
+      <c r="B1735">
+        <v>1879</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F1735" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1735" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1735" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1735">
+        <v>47</v>
+      </c>
+      <c r="J1735" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1735" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1736">
+        <v>41</v>
+      </c>
+      <c r="B1736">
+        <v>1879</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F1736" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1736" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1736" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1736">
+        <v>47</v>
+      </c>
+      <c r="J1736" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1736" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1737">
+        <v>41</v>
+      </c>
+      <c r="B1737">
+        <v>1879</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F1737" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1737" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1737" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1737">
+        <v>47</v>
+      </c>
+      <c r="J1737" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1737" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1738">
+        <v>41</v>
+      </c>
+      <c r="B1738">
+        <v>1879</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F1738" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1738" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1738" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1738">
+        <v>47</v>
+      </c>
+      <c r="J1738" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1738" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1739">
+        <v>41</v>
+      </c>
+      <c r="B1739">
+        <v>1879</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F1739" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1739" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1739" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1739">
+        <v>47</v>
+      </c>
+      <c r="J1739" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1739" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1740">
+        <v>41</v>
+      </c>
+      <c r="B1740">
+        <v>1879</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>1752</v>
+      </c>
+      <c r="F1740" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1740" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1740" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1740">
+        <v>47</v>
+      </c>
+      <c r="J1740" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1740" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1741">
+        <v>41</v>
+      </c>
+      <c r="B1741">
+        <v>1879</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F1741" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1741" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1741" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1741">
+        <v>47</v>
+      </c>
+      <c r="J1741" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1741" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1742">
+        <v>41</v>
+      </c>
+      <c r="B1742">
+        <v>1879</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>1754</v>
+      </c>
+      <c r="F1742" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1742" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1742" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1742">
+        <v>47</v>
+      </c>
+      <c r="J1742" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1742" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1743">
+        <v>41</v>
+      </c>
+      <c r="B1743">
+        <v>1879</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F1743" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1743" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1743" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1743">
+        <v>47</v>
+      </c>
+      <c r="J1743" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1743" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1744">
+        <v>41</v>
+      </c>
+      <c r="B1744">
+        <v>1879</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F1744" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1744" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1744" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1744">
+        <v>47</v>
+      </c>
+      <c r="J1744" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1744" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1745">
+        <v>41</v>
+      </c>
+      <c r="B1745">
+        <v>1879</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F1745" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1745" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1745" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1745">
+        <v>47</v>
+      </c>
+      <c r="J1745" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1745" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1746">
+        <v>41</v>
+      </c>
+      <c r="B1746">
+        <v>1879</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F1746" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1746" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1746" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1746">
+        <v>47</v>
+      </c>
+      <c r="J1746" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1746" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1747">
+        <v>41</v>
+      </c>
+      <c r="B1747">
+        <v>1879</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F1747" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1747" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1747" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1747">
+        <v>47</v>
+      </c>
+      <c r="J1747" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1747" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1748">
+        <v>41</v>
+      </c>
+      <c r="B1748">
+        <v>1879</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F1748" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1748" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1748" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1748">
+        <v>47</v>
+      </c>
+      <c r="J1748" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1748" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1749">
+        <v>41</v>
+      </c>
+      <c r="B1749">
+        <v>1879</v>
+      </c>
+      <c r="C1749" t="s">
+        <v>1761</v>
+      </c>
+      <c r="F1749" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1749" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1749" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1749">
+        <v>47</v>
+      </c>
+      <c r="J1749" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1749" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1750">
+        <v>41</v>
+      </c>
+      <c r="B1750">
+        <v>1879</v>
+      </c>
+      <c r="C1750" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F1750" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1750" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1750" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1750">
+        <v>47</v>
+      </c>
+      <c r="J1750" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1750" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1751">
+        <v>41</v>
+      </c>
+      <c r="B1751">
+        <v>1879</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F1751" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1751" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1751" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1751">
+        <v>47</v>
+      </c>
+      <c r="J1751" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1751" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1752">
+        <v>41</v>
+      </c>
+      <c r="B1752">
+        <v>1879</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F1752" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1752" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1752" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1752">
+        <v>47</v>
+      </c>
+      <c r="J1752" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1752" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1753">
+        <v>41</v>
+      </c>
+      <c r="B1753">
+        <v>1879</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F1753" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1753" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1753" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1753">
+        <v>47</v>
+      </c>
+      <c r="J1753" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1753" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1754">
+        <v>41</v>
+      </c>
+      <c r="B1754">
+        <v>1879</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>1766</v>
+      </c>
+      <c r="F1754" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1754" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1754" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1754">
+        <v>47</v>
+      </c>
+      <c r="J1754" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1754" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1755">
+        <v>41</v>
+      </c>
+      <c r="B1755">
+        <v>1879</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D1755" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E1755" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F1755" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1755" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1755" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1755">
+        <v>47</v>
+      </c>
+      <c r="J1755" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1755" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1756">
+        <v>41</v>
+      </c>
+      <c r="B1756">
+        <v>1879</v>
+      </c>
+      <c r="C1756" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F1756" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1756" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1756" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1756">
+        <v>47</v>
+      </c>
+      <c r="J1756" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1756" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1757">
+        <v>41</v>
+      </c>
+      <c r="B1757">
+        <v>1879</v>
+      </c>
+      <c r="C1757" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F1757" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1757" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1757" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1757">
+        <v>47</v>
+      </c>
+      <c r="J1757" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1757" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1758">
+        <v>41</v>
+      </c>
+      <c r="B1758">
+        <v>1879</v>
+      </c>
+      <c r="C1758" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F1758" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1758" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1758" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1758">
+        <v>47</v>
+      </c>
+      <c r="J1758" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1758" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1759">
+        <v>41</v>
+      </c>
+      <c r="B1759">
+        <v>1879</v>
+      </c>
+      <c r="C1759" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F1759" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1759" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1759" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1759">
+        <v>47</v>
+      </c>
+      <c r="J1759" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1759" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1760">
+        <v>41</v>
+      </c>
+      <c r="B1760">
+        <v>1879</v>
+      </c>
+      <c r="C1760" t="s">
+        <v>1774</v>
+      </c>
+      <c r="F1760" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1760" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1760" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1760">
+        <v>47</v>
+      </c>
+      <c r="J1760" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1760" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1761">
+        <v>41</v>
+      </c>
+      <c r="B1761">
+        <v>1879</v>
+      </c>
+      <c r="C1761" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F1761" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1761" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1761" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1761">
+        <v>47</v>
+      </c>
+      <c r="J1761" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1761" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1762">
+        <v>41</v>
+      </c>
+      <c r="B1762">
+        <v>1879</v>
+      </c>
+      <c r="C1762" t="s">
+        <v>1776</v>
+      </c>
+      <c r="F1762" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1762" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1762" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1762">
+        <v>47</v>
+      </c>
+      <c r="J1762" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1762" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1763">
+        <v>41</v>
+      </c>
+      <c r="B1763">
+        <v>1879</v>
+      </c>
+      <c r="C1763" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F1763" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1763" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1763" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1763">
+        <v>47</v>
+      </c>
+      <c r="J1763" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1763" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1764">
+        <v>41</v>
+      </c>
+      <c r="B1764">
+        <v>1879</v>
+      </c>
+      <c r="C1764" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F1764" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1764" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1764" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1764">
+        <v>47</v>
+      </c>
+      <c r="J1764" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1764" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1765">
+        <v>41</v>
+      </c>
+      <c r="B1765">
+        <v>1879</v>
+      </c>
+      <c r="C1765" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F1765" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1765" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1765" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1765">
+        <v>47</v>
+      </c>
+      <c r="J1765" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1765" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1766">
+        <v>41</v>
+      </c>
+      <c r="B1766">
+        <v>1879</v>
+      </c>
+      <c r="C1766" t="s">
+        <v>1780</v>
+      </c>
+      <c r="F1766" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G1766" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1766" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1766">
+        <v>47</v>
+      </c>
+      <c r="J1766" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1766" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>